<commit_message>
penambahan kota dan negara di tour package
</commit_message>
<xml_diff>
--- a/document/Main Page.xlsx
+++ b/document/Main Page.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="93">
   <si>
     <t>LOGO</t>
   </si>
@@ -294,6 +294,9 @@
   <si>
     <t xml:space="preserve">pake bar </t>
   </si>
+  <si>
+    <t>v</t>
+  </si>
 </sst>
 </file>
 
@@ -332,7 +335,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +345,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -490,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -528,6 +537,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1994,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB113"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AT18" sqref="AT18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,18 +2352,27 @@
       <c r="V10" s="23"/>
       <c r="W10" s="23"/>
       <c r="X10" s="24"/>
-      <c r="Z10" s="22" t="s">
+      <c r="Z10" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA10" s="40"/>
+      <c r="AB10" s="40"/>
+      <c r="AC10" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD10" s="42"/>
+      <c r="AE10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="AA10" s="23"/>
-      <c r="AB10" s="24" t="s">
+      <c r="AF10" s="23"/>
+      <c r="AG10" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="AD10" s="27" t="s">
+      <c r="AI10" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AE10" s="25"/>
-      <c r="AF10" s="26"/>
+      <c r="AJ10" s="25"/>
+      <c r="AK10" s="26"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AD11" s="16"/>
@@ -11050,8 +11074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AI15" sqref="AI15"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="AT83" sqref="AT83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13451,14 +13475,18 @@
       <c r="AN75" s="5"/>
       <c r="AO75" s="5"/>
       <c r="AP75" s="5"/>
-      <c r="AQ75" s="5"/>
-      <c r="AR75" s="5"/>
-      <c r="AS75" s="5"/>
-      <c r="AT75" s="5"/>
-      <c r="AU75" s="5"/>
-      <c r="AV75" s="5"/>
-      <c r="AW75" s="5"/>
-      <c r="AX75" s="5"/>
+      <c r="AQ75" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="AR75" s="37"/>
+      <c r="AS75" s="37"/>
+      <c r="AT75" s="37"/>
+      <c r="AU75" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="AV75" s="37"/>
+      <c r="AW75" s="37"/>
+      <c r="AX75" s="37"/>
       <c r="AZ75" s="5"/>
       <c r="BA75" s="5"/>
       <c r="BB75" s="5"/>
@@ -13514,14 +13542,14 @@
       </c>
       <c r="AO76" s="5"/>
       <c r="AP76" s="5"/>
-      <c r="AQ76" s="5"/>
-      <c r="AR76" s="5"/>
-      <c r="AS76" s="5"/>
-      <c r="AT76" s="5"/>
-      <c r="AU76" s="5"/>
-      <c r="AV76" s="5"/>
-      <c r="AW76" s="5"/>
-      <c r="AX76" s="5"/>
+      <c r="AQ76" s="38"/>
+      <c r="AR76" s="38"/>
+      <c r="AS76" s="38"/>
+      <c r="AT76" s="37"/>
+      <c r="AU76" s="38"/>
+      <c r="AV76" s="38"/>
+      <c r="AW76" s="38"/>
+      <c r="AX76" s="37"/>
       <c r="AZ76" s="5"/>
       <c r="BA76" s="5"/>
       <c r="BB76" s="5"/>

</xml_diff>

<commit_message>
penambahan spec ada di warna kuning
</commit_message>
<xml_diff>
--- a/document/Main Page.xlsx
+++ b/document/Main Page.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="1" r:id="rId1"/>
     <sheet name="Traveller" sheetId="2" r:id="rId2"/>
     <sheet name="Tour" sheetId="3" r:id="rId3"/>
     <sheet name="Admin" sheetId="4" r:id="rId4"/>
+    <sheet name="public vendor" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="113">
   <si>
     <t>LOGO</t>
   </si>
@@ -297,6 +298,66 @@
   <si>
     <t>v</t>
   </si>
+  <si>
+    <t>Dialog register</t>
+  </si>
+  <si>
+    <t>ini untuk register vendor / traveller sama aky gini bentuknya</t>
+  </si>
+  <si>
+    <t>Kontent yang ada disini</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>list itenary dari si tour</t>
+  </si>
+  <si>
+    <t>(isi listnya harus berupa category,price,negara,kota,periode</t>
+  </si>
+  <si>
+    <t>album si tour</t>
+  </si>
+  <si>
+    <t>Periode</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Pax</t>
+  </si>
+  <si>
+    <t>disini user hanya bs lihat saja atau tekan tombol ask itenary,send message dan save as favorit</t>
+  </si>
+  <si>
+    <t>ada tombol ask itenary dan save untuk jadi favorit tour,message</t>
+  </si>
+  <si>
+    <t>di bagian itenary ada kaya semacam search khusus diitenary untuk tour tersebut, bukan yg sticky</t>
+  </si>
+  <si>
+    <t>contoh:</t>
+  </si>
+  <si>
+    <t>Periode from</t>
+  </si>
+  <si>
+    <t>Negara</t>
+  </si>
+  <si>
+    <t>Kota</t>
+  </si>
+  <si>
+    <t>ini hanya akan reset dihalaman tabnya/halaman itenary bukan semua</t>
+  </si>
+  <si>
+    <t>harus ad aprofile untuk dari si tour(nama tour,nomor tlp,alamat),ini akan selalu tampil walaupun user pilih album atau ganti ke itenary</t>
+  </si>
 </sst>
 </file>
 
@@ -499,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -543,6 +604,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,13 +788,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>114</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2007,10 +2082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB113"/>
+  <dimension ref="A1:BB127"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AT18" sqref="AT18"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,859 +3956,467 @@
       <c r="Y60" s="2"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="67" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="s">
+    <row r="64" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="44"/>
+      <c r="B65" s="45"/>
+      <c r="C65" s="45"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="45"/>
+      <c r="I65" s="45"/>
+      <c r="J65" s="45"/>
+      <c r="K65" s="45"/>
+      <c r="L65" s="45"/>
+      <c r="M65" s="45"/>
+      <c r="N65" s="45"/>
+      <c r="O65" s="45"/>
+      <c r="P65" s="45"/>
+      <c r="Q65" s="45"/>
+      <c r="R65" s="45"/>
+      <c r="S65" s="45"/>
+      <c r="T65" s="45"/>
+      <c r="U65" s="45"/>
+      <c r="V65" s="45"/>
+      <c r="W65" s="45"/>
+      <c r="X65" s="45"/>
+      <c r="Y65" s="45"/>
+      <c r="Z65" s="46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="47" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
+      <c r="K66" s="37"/>
+      <c r="L66" s="37"/>
+      <c r="M66" s="37"/>
+      <c r="N66" s="37"/>
+      <c r="O66" s="37"/>
+      <c r="P66" s="37"/>
+      <c r="Q66" s="37"/>
+      <c r="R66" s="37"/>
+      <c r="S66" s="37"/>
+      <c r="T66" s="37"/>
+      <c r="U66" s="37"/>
+      <c r="V66" s="37"/>
+      <c r="W66" s="37"/>
+      <c r="X66" s="37"/>
+      <c r="Y66" s="37"/>
+      <c r="Z66" s="48"/>
+    </row>
+    <row r="67" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="49"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="38"/>
+      <c r="E67" s="38"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
+      <c r="K67" s="38"/>
+      <c r="L67" s="38"/>
+      <c r="M67" s="38"/>
+      <c r="N67" s="38"/>
+      <c r="O67" s="38"/>
+      <c r="P67" s="38"/>
+      <c r="Q67" s="38"/>
+      <c r="R67" s="38"/>
+      <c r="S67" s="38"/>
+      <c r="T67" s="38"/>
+      <c r="U67" s="38"/>
+      <c r="V67" s="38"/>
+      <c r="W67" s="38"/>
+      <c r="X67" s="38"/>
+      <c r="Y67" s="38"/>
+      <c r="Z67" s="50"/>
+    </row>
+    <row r="68" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="51"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="37"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="37"/>
+      <c r="M68" s="37"/>
+      <c r="N68" s="37"/>
+      <c r="O68" s="37"/>
+      <c r="P68" s="37"/>
+      <c r="Q68" s="37"/>
+      <c r="R68" s="37"/>
+      <c r="S68" s="37"/>
+      <c r="T68" s="37"/>
+      <c r="U68" s="37"/>
+      <c r="V68" s="37"/>
+      <c r="W68" s="37"/>
+      <c r="X68" s="37"/>
+      <c r="Y68" s="37"/>
+      <c r="Z68" s="48"/>
+      <c r="AH68" s="42" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B69" s="37"/>
+      <c r="C69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
+      <c r="L69" s="37"/>
+      <c r="M69" s="37"/>
+      <c r="N69" s="37"/>
+      <c r="O69" s="37"/>
+      <c r="P69" s="37"/>
+      <c r="Q69" s="37"/>
+      <c r="R69" s="37"/>
+      <c r="S69" s="37"/>
+      <c r="T69" s="37"/>
+      <c r="U69" s="37"/>
+      <c r="V69" s="37"/>
+      <c r="W69" s="37"/>
+      <c r="X69" s="37"/>
+      <c r="Y69" s="37"/>
+      <c r="Z69" s="48"/>
+    </row>
+    <row r="70" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="49"/>
+      <c r="B70" s="38"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="38"/>
+      <c r="G70" s="38"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
+      <c r="J70" s="38"/>
+      <c r="K70" s="38"/>
+      <c r="L70" s="37"/>
+      <c r="M70" s="37"/>
+      <c r="N70" s="37"/>
+      <c r="O70" s="37"/>
+      <c r="P70" s="37"/>
+      <c r="Q70" s="37"/>
+      <c r="R70" s="37"/>
+      <c r="S70" s="37"/>
+      <c r="T70" s="37"/>
+      <c r="U70" s="37"/>
+      <c r="V70" s="37"/>
+      <c r="W70" s="37"/>
+      <c r="X70" s="37"/>
+      <c r="Y70" s="37"/>
+      <c r="Z70" s="48"/>
+    </row>
+    <row r="71" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="51"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="37"/>
+      <c r="K71" s="37"/>
+      <c r="L71" s="37"/>
+      <c r="M71" s="37"/>
+      <c r="N71" s="37"/>
+      <c r="O71" s="37"/>
+      <c r="P71" s="37"/>
+      <c r="Q71" s="37"/>
+      <c r="R71" s="37"/>
+      <c r="S71" s="37"/>
+      <c r="T71" s="37"/>
+      <c r="U71" s="37"/>
+      <c r="V71" s="37"/>
+      <c r="W71" s="37"/>
+      <c r="X71" s="37"/>
+      <c r="Y71" s="37"/>
+      <c r="Z71" s="48"/>
+    </row>
+    <row r="72" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="37"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="37"/>
+      <c r="K72" s="37"/>
+      <c r="L72" s="37"/>
+      <c r="M72" s="37"/>
+      <c r="N72" s="37"/>
+      <c r="O72" s="37"/>
+      <c r="P72" s="37"/>
+      <c r="Q72" s="37"/>
+      <c r="R72" s="37"/>
+      <c r="S72" s="37"/>
+      <c r="T72" s="37"/>
+      <c r="U72" s="37"/>
+      <c r="V72" s="37"/>
+      <c r="W72" s="37"/>
+      <c r="X72" s="37"/>
+      <c r="Y72" s="37"/>
+      <c r="Z72" s="48"/>
+    </row>
+    <row r="73" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="49"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="38"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
+      <c r="J73" s="38"/>
+      <c r="K73" s="38"/>
+      <c r="L73" s="37"/>
+      <c r="M73" s="37"/>
+      <c r="N73" s="37"/>
+      <c r="O73" s="37"/>
+      <c r="P73" s="37"/>
+      <c r="Q73" s="37"/>
+      <c r="R73" s="37"/>
+      <c r="S73" s="37"/>
+      <c r="T73" s="37"/>
+      <c r="U73" s="37"/>
+      <c r="V73" s="37"/>
+      <c r="W73" s="37"/>
+      <c r="X73" s="37"/>
+      <c r="Y73" s="37"/>
+      <c r="Z73" s="48"/>
+    </row>
+    <row r="74" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="51"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="37"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="37"/>
+      <c r="K74" s="37"/>
+      <c r="L74" s="37"/>
+      <c r="M74" s="37"/>
+      <c r="N74" s="37"/>
+      <c r="O74" s="37"/>
+      <c r="P74" s="37"/>
+      <c r="Q74" s="37"/>
+      <c r="R74" s="37"/>
+      <c r="S74" s="37"/>
+      <c r="T74" s="37"/>
+      <c r="U74" s="37"/>
+      <c r="V74" s="37"/>
+      <c r="W74" s="37"/>
+      <c r="X74" s="37"/>
+      <c r="Y74" s="37"/>
+      <c r="Z74" s="48"/>
+    </row>
+    <row r="75" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="51"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="37"/>
+      <c r="L75" s="37"/>
+      <c r="M75" s="37"/>
+      <c r="N75" s="37"/>
+      <c r="O75" s="37"/>
+      <c r="P75" s="37"/>
+      <c r="Q75" s="37"/>
+      <c r="R75" s="37"/>
+      <c r="S75" s="37"/>
+      <c r="T75" s="37"/>
+      <c r="U75" s="37"/>
+      <c r="V75" s="37"/>
+      <c r="W75" s="37"/>
+      <c r="X75" s="37"/>
+      <c r="Y75" s="37"/>
+      <c r="Z75" s="48"/>
+    </row>
+    <row r="76" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="40"/>
+      <c r="C76" s="40"/>
+      <c r="D76" s="41"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="37"/>
+      <c r="L76" s="37"/>
+      <c r="M76" s="37"/>
+      <c r="N76" s="37"/>
+      <c r="O76" s="37"/>
+      <c r="P76" s="37"/>
+      <c r="Q76" s="37"/>
+      <c r="R76" s="37"/>
+      <c r="S76" s="37"/>
+      <c r="T76" s="37"/>
+      <c r="U76" s="37"/>
+      <c r="V76" s="37"/>
+      <c r="W76" s="37"/>
+      <c r="X76" s="37"/>
+      <c r="Y76" s="37"/>
+      <c r="Z76" s="48"/>
+    </row>
+    <row r="77" spans="1:34" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="38"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="38"/>
+      <c r="E77" s="38"/>
+      <c r="F77" s="38"/>
+      <c r="G77" s="38"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="38"/>
+      <c r="K77" s="38"/>
+      <c r="L77" s="38"/>
+      <c r="M77" s="38"/>
+      <c r="N77" s="38"/>
+      <c r="O77" s="38"/>
+      <c r="P77" s="38"/>
+      <c r="Q77" s="38"/>
+      <c r="R77" s="38"/>
+      <c r="S77" s="38"/>
+      <c r="T77" s="38"/>
+      <c r="U77" s="38"/>
+      <c r="V77" s="38"/>
+      <c r="W77" s="38"/>
+      <c r="X77" s="38"/>
+      <c r="Y77" s="38"/>
+      <c r="Z77" s="50"/>
+    </row>
+    <row r="81" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A81" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="AC67" s="21" t="s">
+      <c r="AC81" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A68" s="32"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="8"/>
-      <c r="M68" s="8"/>
-      <c r="N68" s="8"/>
-      <c r="O68" s="8"/>
-      <c r="P68" s="8"/>
-      <c r="Q68" s="8"/>
-      <c r="R68" s="8"/>
-      <c r="S68" s="8"/>
-      <c r="T68" s="8"/>
-      <c r="U68" s="8"/>
-      <c r="V68" s="8"/>
-      <c r="W68" s="8"/>
-      <c r="X68" s="8"/>
-      <c r="Y68" s="8"/>
-      <c r="Z68" s="7"/>
-      <c r="AC68" s="32"/>
-      <c r="AD68" s="8"/>
-      <c r="AE68" s="7"/>
-      <c r="AF68" s="8"/>
-      <c r="AG68" s="8"/>
-      <c r="AH68" s="8"/>
-      <c r="AI68" s="8"/>
-      <c r="AJ68" s="8"/>
-      <c r="AK68" s="8"/>
-      <c r="AL68" s="8"/>
-      <c r="AM68" s="8"/>
-      <c r="AN68" s="8"/>
-      <c r="AO68" s="8"/>
-      <c r="AP68" s="8"/>
-      <c r="AQ68" s="8"/>
-      <c r="AR68" s="8"/>
-      <c r="AS68" s="8"/>
-      <c r="AT68" s="8"/>
-      <c r="AU68" s="8"/>
-      <c r="AV68" s="8"/>
-      <c r="AW68" s="8"/>
-      <c r="AX68" s="8"/>
-      <c r="AY68" s="8"/>
-      <c r="AZ68" s="8"/>
-      <c r="BA68" s="8"/>
-      <c r="BB68" s="7"/>
-    </row>
-    <row r="69" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+    <row r="82" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A82" s="32"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="8"/>
+      <c r="M82" s="8"/>
+      <c r="N82" s="8"/>
+      <c r="O82" s="8"/>
+      <c r="P82" s="8"/>
+      <c r="Q82" s="8"/>
+      <c r="R82" s="8"/>
+      <c r="S82" s="8"/>
+      <c r="T82" s="8"/>
+      <c r="U82" s="8"/>
+      <c r="V82" s="8"/>
+      <c r="W82" s="8"/>
+      <c r="X82" s="8"/>
+      <c r="Y82" s="8"/>
+      <c r="Z82" s="7"/>
+      <c r="AC82" s="32"/>
+      <c r="AD82" s="8"/>
+      <c r="AE82" s="7"/>
+      <c r="AF82" s="8"/>
+      <c r="AG82" s="8"/>
+      <c r="AH82" s="8"/>
+      <c r="AI82" s="8"/>
+      <c r="AJ82" s="8"/>
+      <c r="AK82" s="8"/>
+      <c r="AL82" s="8"/>
+      <c r="AM82" s="8"/>
+      <c r="AN82" s="8"/>
+      <c r="AO82" s="8"/>
+      <c r="AP82" s="8"/>
+      <c r="AQ82" s="8"/>
+      <c r="AR82" s="8"/>
+      <c r="AS82" s="8"/>
+      <c r="AT82" s="8"/>
+      <c r="AU82" s="8"/>
+      <c r="AV82" s="8"/>
+      <c r="AW82" s="8"/>
+      <c r="AX82" s="8"/>
+      <c r="AY82" s="8"/>
+      <c r="AZ82" s="8"/>
+      <c r="BA82" s="8"/>
+      <c r="BB82" s="7"/>
+    </row>
+    <row r="83" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A83" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B69" s="5"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="30"/>
-      <c r="J69" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="T69" s="5"/>
-      <c r="U69" s="5"/>
-      <c r="V69" s="5"/>
-      <c r="W69" s="5"/>
-      <c r="X69" s="5"/>
-      <c r="Y69" s="5"/>
-      <c r="Z69" s="4"/>
-      <c r="AC69" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD69" s="5"/>
-      <c r="AE69" s="4"/>
-      <c r="AF69" s="5"/>
-      <c r="AG69" s="5"/>
-      <c r="AH69" s="5"/>
-      <c r="AI69" s="5"/>
-      <c r="AJ69" s="5"/>
-      <c r="AK69" s="30"/>
-      <c r="AL69" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM69" s="5"/>
-      <c r="AN69" s="5"/>
-      <c r="AO69" s="5"/>
-      <c r="AP69" s="5"/>
-      <c r="AQ69" s="5"/>
-      <c r="AR69" s="5"/>
-      <c r="AS69" s="5"/>
-      <c r="AT69" s="5"/>
-      <c r="AU69" s="5"/>
-      <c r="AV69" s="5"/>
-      <c r="AW69" s="5"/>
-      <c r="AX69" s="5"/>
-      <c r="AY69" s="5"/>
-      <c r="AZ69" s="5"/>
-      <c r="BA69" s="5"/>
-      <c r="BB69" s="4"/>
-    </row>
-    <row r="70" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-      <c r="K70" s="2"/>
-      <c r="L70" s="2"/>
-      <c r="M70" s="2"/>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" s="2"/>
-      <c r="Q70" s="2"/>
-      <c r="R70" s="2"/>
-      <c r="S70" s="2"/>
-      <c r="T70" s="2"/>
-      <c r="U70" s="2"/>
-      <c r="V70" s="2"/>
-      <c r="W70" s="2"/>
-      <c r="X70" s="2"/>
-      <c r="Y70" s="2"/>
-      <c r="Z70" s="1"/>
-      <c r="AC70" s="3"/>
-      <c r="AD70" s="2"/>
-      <c r="AE70" s="1"/>
-      <c r="AF70" s="2"/>
-      <c r="AG70" s="2"/>
-      <c r="AH70" s="2"/>
-      <c r="AI70" s="2"/>
-      <c r="AJ70" s="2"/>
-      <c r="AK70" s="2"/>
-      <c r="AL70" s="2"/>
-      <c r="AM70" s="2"/>
-      <c r="AN70" s="2"/>
-      <c r="AO70" s="2"/>
-      <c r="AP70" s="2"/>
-      <c r="AQ70" s="2"/>
-      <c r="AR70" s="2"/>
-      <c r="AS70" s="2"/>
-      <c r="AT70" s="2"/>
-      <c r="AU70" s="2"/>
-      <c r="AV70" s="2"/>
-      <c r="AW70" s="2"/>
-      <c r="AX70" s="2"/>
-      <c r="AY70" s="2"/>
-      <c r="AZ70" s="2"/>
-      <c r="BA70" s="2"/>
-      <c r="BB70" s="1"/>
-    </row>
-    <row r="71" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A71" s="9"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
-      <c r="L71" s="8"/>
-      <c r="M71" s="8"/>
-      <c r="N71" s="8"/>
-      <c r="O71" s="8"/>
-      <c r="P71" s="8"/>
-      <c r="Q71" s="8"/>
-      <c r="R71" s="8"/>
-      <c r="S71" s="8"/>
-      <c r="T71" s="8"/>
-      <c r="U71" s="8"/>
-      <c r="V71" s="8"/>
-      <c r="W71" s="8"/>
-      <c r="X71" s="8"/>
-      <c r="Y71" s="8"/>
-      <c r="Z71" s="7"/>
-      <c r="AC71" s="9"/>
-      <c r="AD71" s="8"/>
-      <c r="AE71" s="8"/>
-      <c r="AF71" s="8"/>
-      <c r="AG71" s="8"/>
-      <c r="AH71" s="8"/>
-      <c r="AI71" s="8"/>
-      <c r="AJ71" s="8"/>
-      <c r="AK71" s="8"/>
-      <c r="AL71" s="8"/>
-      <c r="AM71" s="8"/>
-      <c r="AN71" s="8"/>
-      <c r="AO71" s="8"/>
-      <c r="AP71" s="8"/>
-      <c r="AQ71" s="8"/>
-      <c r="AR71" s="8"/>
-      <c r="AS71" s="8"/>
-      <c r="AT71" s="8"/>
-      <c r="AU71" s="8"/>
-      <c r="AV71" s="8"/>
-      <c r="AW71" s="8"/>
-      <c r="AX71" s="8"/>
-      <c r="AY71" s="8"/>
-      <c r="AZ71" s="8"/>
-      <c r="BA71" s="8"/>
-      <c r="BB71" s="7"/>
-    </row>
-    <row r="72" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-      <c r="K72" s="5"/>
-      <c r="L72" s="9"/>
-      <c r="M72" s="8"/>
-      <c r="N72" s="8"/>
-      <c r="O72" s="8"/>
-      <c r="P72" s="8"/>
-      <c r="Q72" s="7"/>
-      <c r="R72" s="5"/>
-      <c r="S72" s="5"/>
-      <c r="T72" s="5"/>
-      <c r="U72" s="5"/>
-      <c r="V72" s="5"/>
-      <c r="W72" s="5"/>
-      <c r="X72" s="5"/>
-      <c r="Y72" s="5"/>
-      <c r="Z72" s="4"/>
-      <c r="AC72" s="11"/>
-      <c r="AD72" s="5"/>
-      <c r="AE72" s="5"/>
-      <c r="AF72" s="5"/>
-      <c r="AG72" s="5"/>
-      <c r="AH72" s="5"/>
-      <c r="AI72" s="5"/>
-      <c r="AJ72" s="5"/>
-      <c r="AK72" s="5"/>
-      <c r="AL72" s="5"/>
-      <c r="AM72" s="5"/>
-      <c r="AN72" s="9"/>
-      <c r="AO72" s="8"/>
-      <c r="AP72" s="8"/>
-      <c r="AQ72" s="8"/>
-      <c r="AR72" s="8"/>
-      <c r="AS72" s="7"/>
-      <c r="AT72" s="5"/>
-      <c r="AU72" s="5"/>
-      <c r="AV72" s="5"/>
-      <c r="AW72" s="5"/>
-      <c r="AX72" s="5"/>
-      <c r="AY72" s="5"/>
-      <c r="AZ72" s="5"/>
-      <c r="BA72" s="5"/>
-      <c r="BB72" s="4"/>
-    </row>
-    <row r="73" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="5"/>
-      <c r="L73" s="11"/>
-      <c r="M73" s="5"/>
-      <c r="N73" s="5"/>
-      <c r="O73" s="5"/>
-      <c r="P73" s="5"/>
-      <c r="Q73" s="4"/>
-      <c r="R73" s="5"/>
-      <c r="S73" s="5"/>
-      <c r="T73" s="5"/>
-      <c r="U73" s="5"/>
-      <c r="V73" s="5"/>
-      <c r="W73" s="5"/>
-      <c r="X73" s="5"/>
-      <c r="Y73" s="5"/>
-      <c r="Z73" s="4"/>
-      <c r="AC73" s="11"/>
-      <c r="AD73" s="5"/>
-      <c r="AE73" s="5"/>
-      <c r="AF73" s="5"/>
-      <c r="AG73" s="5"/>
-      <c r="AH73" s="5"/>
-      <c r="AI73" s="5"/>
-      <c r="AJ73" s="5"/>
-      <c r="AK73" s="5"/>
-      <c r="AL73" s="5"/>
-      <c r="AM73" s="5"/>
-      <c r="AN73" s="11"/>
-      <c r="AO73" s="5"/>
-      <c r="AP73" s="5"/>
-      <c r="AQ73" s="5"/>
-      <c r="AR73" s="5"/>
-      <c r="AS73" s="4"/>
-      <c r="AT73" s="5"/>
-      <c r="AU73" s="5"/>
-      <c r="AV73" s="5"/>
-      <c r="AW73" s="5"/>
-      <c r="AX73" s="5"/>
-      <c r="AY73" s="5"/>
-      <c r="AZ73" s="5"/>
-      <c r="BA73" s="5"/>
-      <c r="BB73" s="4"/>
-    </row>
-    <row r="74" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="11"/>
-      <c r="M74" s="5"/>
-      <c r="N74" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O74" s="5"/>
-      <c r="P74" s="5"/>
-      <c r="Q74" s="4"/>
-      <c r="R74" s="5"/>
-      <c r="S74" s="5"/>
-      <c r="T74" s="5"/>
-      <c r="U74" s="5"/>
-      <c r="V74" s="5"/>
-      <c r="W74" s="5"/>
-      <c r="X74" s="5"/>
-      <c r="Y74" s="5"/>
-      <c r="Z74" s="4"/>
-      <c r="AC74" s="11"/>
-      <c r="AD74" s="5"/>
-      <c r="AE74" s="5"/>
-      <c r="AF74" s="5"/>
-      <c r="AG74" s="5"/>
-      <c r="AH74" s="5"/>
-      <c r="AI74" s="5"/>
-      <c r="AJ74" s="5"/>
-      <c r="AK74" s="5"/>
-      <c r="AL74" s="5"/>
-      <c r="AM74" s="5"/>
-      <c r="AN74" s="11"/>
-      <c r="AO74" s="5"/>
-      <c r="AP74" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ74" s="5"/>
-      <c r="AR74" s="5"/>
-      <c r="AS74" s="4"/>
-      <c r="AT74" s="5"/>
-      <c r="AU74" s="5"/>
-      <c r="AV74" s="5"/>
-      <c r="AW74" s="5"/>
-      <c r="AX74" s="5"/>
-      <c r="AY74" s="5"/>
-      <c r="AZ74" s="5"/>
-      <c r="BA74" s="5"/>
-      <c r="BB74" s="4"/>
-    </row>
-    <row r="75" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-      <c r="K75" s="5"/>
-      <c r="L75" s="11"/>
-      <c r="M75" s="5"/>
-      <c r="N75" s="5"/>
-      <c r="O75" s="5"/>
-      <c r="P75" s="5"/>
-      <c r="Q75" s="4"/>
-      <c r="R75" s="5"/>
-      <c r="S75" s="5"/>
-      <c r="T75" s="5"/>
-      <c r="U75" s="5"/>
-      <c r="V75" s="5"/>
-      <c r="W75" s="5"/>
-      <c r="X75" s="5"/>
-      <c r="Y75" s="5"/>
-      <c r="Z75" s="4"/>
-      <c r="AC75" s="11"/>
-      <c r="AD75" s="5"/>
-      <c r="AE75" s="5"/>
-      <c r="AF75" s="5"/>
-      <c r="AG75" s="5"/>
-      <c r="AH75" s="5"/>
-      <c r="AI75" s="5"/>
-      <c r="AJ75" s="5"/>
-      <c r="AK75" s="5"/>
-      <c r="AL75" s="5"/>
-      <c r="AM75" s="5"/>
-      <c r="AN75" s="11"/>
-      <c r="AO75" s="5"/>
-      <c r="AP75" s="5"/>
-      <c r="AQ75" s="5"/>
-      <c r="AR75" s="5"/>
-      <c r="AS75" s="4"/>
-      <c r="AT75" s="5"/>
-      <c r="AU75" s="5"/>
-      <c r="AV75" s="5"/>
-      <c r="AW75" s="5"/>
-      <c r="AX75" s="5"/>
-      <c r="AY75" s="5"/>
-      <c r="AZ75" s="5"/>
-      <c r="BA75" s="5"/>
-      <c r="BB75" s="4"/>
-    </row>
-    <row r="76" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-      <c r="K76" s="5"/>
-      <c r="L76" s="11"/>
-      <c r="M76" s="5"/>
-      <c r="N76" s="5"/>
-      <c r="O76" s="5"/>
-      <c r="P76" s="5"/>
-      <c r="Q76" s="4"/>
-      <c r="R76" s="5"/>
-      <c r="S76" s="5"/>
-      <c r="T76" s="5"/>
-      <c r="U76" s="5"/>
-      <c r="V76" s="5"/>
-      <c r="W76" s="5"/>
-      <c r="X76" s="5"/>
-      <c r="Y76" s="5"/>
-      <c r="Z76" s="4"/>
-      <c r="AC76" s="11"/>
-      <c r="AD76" s="5"/>
-      <c r="AE76" s="5"/>
-      <c r="AF76" s="5"/>
-      <c r="AG76" s="5"/>
-      <c r="AH76" s="5"/>
-      <c r="AI76" s="5"/>
-      <c r="AJ76" s="5"/>
-      <c r="AK76" s="5"/>
-      <c r="AL76" s="5"/>
-      <c r="AM76" s="5"/>
-      <c r="AN76" s="11"/>
-      <c r="AO76" s="5"/>
-      <c r="AP76" s="5"/>
-      <c r="AQ76" s="5"/>
-      <c r="AR76" s="5"/>
-      <c r="AS76" s="4"/>
-      <c r="AT76" s="5"/>
-      <c r="AU76" s="5"/>
-      <c r="AV76" s="5"/>
-      <c r="AW76" s="5"/>
-      <c r="AX76" s="5"/>
-      <c r="AY76" s="5"/>
-      <c r="AZ76" s="5"/>
-      <c r="BA76" s="5"/>
-      <c r="BB76" s="4"/>
-    </row>
-    <row r="77" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A77" s="11"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
-      <c r="K77" s="5"/>
-      <c r="L77" s="3"/>
-      <c r="M77" s="2"/>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="5"/>
-      <c r="S77" s="5"/>
-      <c r="T77" s="5"/>
-      <c r="U77" s="5"/>
-      <c r="V77" s="5"/>
-      <c r="W77" s="5"/>
-      <c r="X77" s="5"/>
-      <c r="Y77" s="5"/>
-      <c r="Z77" s="4"/>
-      <c r="AC77" s="11"/>
-      <c r="AD77" s="5"/>
-      <c r="AE77" s="5"/>
-      <c r="AF77" s="5"/>
-      <c r="AG77" s="5"/>
-      <c r="AH77" s="5"/>
-      <c r="AI77" s="5"/>
-      <c r="AJ77" s="5"/>
-      <c r="AK77" s="5"/>
-      <c r="AL77" s="5"/>
-      <c r="AM77" s="5"/>
-      <c r="AN77" s="3"/>
-      <c r="AO77" s="2"/>
-      <c r="AP77" s="2"/>
-      <c r="AQ77" s="2"/>
-      <c r="AR77" s="2"/>
-      <c r="AS77" s="1"/>
-      <c r="AT77" s="5"/>
-      <c r="AU77" s="5"/>
-      <c r="AV77" s="5"/>
-      <c r="AW77" s="5"/>
-      <c r="AX77" s="5"/>
-      <c r="AY77" s="5"/>
-      <c r="AZ77" s="5"/>
-      <c r="BA77" s="5"/>
-      <c r="BB77" s="4"/>
-    </row>
-    <row r="78" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A78" s="11"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-      <c r="M78" s="5"/>
-      <c r="N78" s="5"/>
-      <c r="O78" s="5"/>
-      <c r="P78" s="5"/>
-      <c r="Q78" s="5"/>
-      <c r="R78" s="5"/>
-      <c r="S78" s="5"/>
-      <c r="T78" s="5"/>
-      <c r="U78" s="5"/>
-      <c r="V78" s="5"/>
-      <c r="W78" s="5"/>
-      <c r="X78" s="5"/>
-      <c r="Y78" s="5"/>
-      <c r="Z78" s="4"/>
-      <c r="AC78" s="11"/>
-      <c r="AD78" s="5"/>
-      <c r="AE78" s="5"/>
-      <c r="AF78" s="5"/>
-      <c r="AG78" s="5"/>
-      <c r="AH78" s="5"/>
-      <c r="AI78" s="5"/>
-      <c r="AJ78" s="5"/>
-      <c r="AK78" s="5"/>
-      <c r="AL78" s="5"/>
-      <c r="AM78" s="5"/>
-      <c r="AN78" s="5"/>
-      <c r="AO78" s="5"/>
-      <c r="AP78" s="5"/>
-      <c r="AQ78" s="5"/>
-      <c r="AR78" s="5"/>
-      <c r="AS78" s="5"/>
-      <c r="AT78" s="5"/>
-      <c r="AU78" s="5"/>
-      <c r="AV78" s="5"/>
-      <c r="AW78" s="5"/>
-      <c r="AX78" s="5"/>
-      <c r="AY78" s="5"/>
-      <c r="AZ78" s="5"/>
-      <c r="BA78" s="5"/>
-      <c r="BB78" s="4"/>
-    </row>
-    <row r="79" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A79" s="11"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
-      <c r="J79" s="5"/>
-      <c r="K79" s="5"/>
-      <c r="L79" s="22"/>
-      <c r="M79" s="23"/>
-      <c r="N79" s="23"/>
-      <c r="O79" s="23"/>
-      <c r="P79" s="24"/>
-      <c r="Q79" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="R79" s="23"/>
-      <c r="S79" s="24"/>
-      <c r="T79" s="5"/>
-      <c r="U79" s="5"/>
-      <c r="V79" s="5"/>
-      <c r="W79" s="5"/>
-      <c r="X79" s="5"/>
-      <c r="Y79" s="5"/>
-      <c r="Z79" s="4"/>
-      <c r="AC79" s="11"/>
-      <c r="AD79" s="5"/>
-      <c r="AE79" s="5"/>
-      <c r="AF79" s="5"/>
-      <c r="AG79" s="5"/>
-      <c r="AH79" s="5"/>
-      <c r="AI79" s="5"/>
-      <c r="AJ79" s="5"/>
-      <c r="AK79" s="5"/>
-      <c r="AL79" s="5"/>
-      <c r="AM79" s="5"/>
-      <c r="AN79" s="22"/>
-      <c r="AO79" s="23"/>
-      <c r="AP79" s="23"/>
-      <c r="AQ79" s="23"/>
-      <c r="AR79" s="24"/>
-      <c r="AS79" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="AT79" s="23"/>
-      <c r="AU79" s="24"/>
-      <c r="AV79" s="5"/>
-      <c r="AW79" s="5"/>
-      <c r="AX79" s="5"/>
-      <c r="AY79" s="5"/>
-      <c r="AZ79" s="5"/>
-      <c r="BA79" s="5"/>
-      <c r="BB79" s="4"/>
-    </row>
-    <row r="80" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5"/>
-      <c r="O80" s="5"/>
-      <c r="P80" s="5"/>
-      <c r="Q80" s="5"/>
-      <c r="R80" s="5"/>
-      <c r="S80" s="5"/>
-      <c r="T80" s="5"/>
-      <c r="U80" s="5"/>
-      <c r="V80" s="5"/>
-      <c r="W80" s="5"/>
-      <c r="X80" s="5"/>
-      <c r="Y80" s="5"/>
-      <c r="Z80" s="4"/>
-      <c r="AC80" s="11"/>
-      <c r="AD80" s="5"/>
-      <c r="AE80" s="5"/>
-      <c r="AF80" s="5"/>
-      <c r="AG80" s="5"/>
-      <c r="AH80" s="5"/>
-      <c r="AI80" s="5"/>
-      <c r="AJ80" s="5"/>
-      <c r="AK80" s="5"/>
-      <c r="AL80" s="5"/>
-      <c r="AM80" s="5"/>
-      <c r="AN80" s="5"/>
-      <c r="AO80" s="5"/>
-      <c r="AP80" s="5"/>
-      <c r="AQ80" s="5"/>
-      <c r="AR80" s="5"/>
-      <c r="AS80" s="5"/>
-      <c r="AT80" s="5"/>
-      <c r="AU80" s="5"/>
-      <c r="AV80" s="5"/>
-      <c r="AW80" s="5"/>
-      <c r="AX80" s="5"/>
-      <c r="AY80" s="5"/>
-      <c r="AZ80" s="5"/>
-      <c r="BA80" s="5"/>
-      <c r="BB80" s="4"/>
-    </row>
-    <row r="81" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
-      <c r="B81" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5"/>
-      <c r="K81" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5"/>
-      <c r="O81" s="5"/>
-      <c r="P81" s="5"/>
-      <c r="Q81" s="5"/>
-      <c r="R81" s="5"/>
-      <c r="S81" s="5"/>
-      <c r="T81" s="5"/>
-      <c r="U81" s="5"/>
-      <c r="V81" s="5"/>
-      <c r="W81" s="5"/>
-      <c r="X81" s="5"/>
-      <c r="Y81" s="5"/>
-      <c r="Z81" s="4"/>
-      <c r="AC81" s="11"/>
-      <c r="AD81" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE81" s="5"/>
-      <c r="AF81" s="5"/>
-      <c r="AG81" s="5"/>
-      <c r="AH81" s="5"/>
-      <c r="AI81" s="5"/>
-      <c r="AJ81" s="5"/>
-      <c r="AK81" s="5"/>
-      <c r="AL81" s="5"/>
-      <c r="AM81" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AN81" s="5"/>
-      <c r="AO81" s="5"/>
-      <c r="AP81" s="5"/>
-      <c r="AQ81" s="5"/>
-      <c r="AR81" s="5"/>
-      <c r="AS81" s="5"/>
-      <c r="AT81" s="5"/>
-      <c r="AU81" s="5"/>
-      <c r="AV81" s="5"/>
-      <c r="AW81" s="5"/>
-      <c r="AX81" s="5"/>
-      <c r="AY81" s="5"/>
-      <c r="AZ81" s="5"/>
-      <c r="BA81" s="5"/>
-      <c r="BB81" s="4"/>
-    </row>
-    <row r="82" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="2"/>
-      <c r="L82" s="2"/>
-      <c r="M82" s="2"/>
-      <c r="N82" s="2"/>
-      <c r="O82" s="2"/>
-      <c r="P82" s="2"/>
-      <c r="Q82" s="2"/>
-      <c r="R82" s="5"/>
-      <c r="S82" s="5"/>
-      <c r="T82" s="5"/>
-      <c r="U82" s="5"/>
-      <c r="V82" s="5"/>
-      <c r="W82" s="5"/>
-      <c r="X82" s="5"/>
-      <c r="Y82" s="5"/>
-      <c r="Z82" s="4"/>
-      <c r="AC82" s="11"/>
-      <c r="AD82" s="2"/>
-      <c r="AE82" s="2"/>
-      <c r="AF82" s="2"/>
-      <c r="AG82" s="2"/>
-      <c r="AH82" s="2"/>
-      <c r="AI82" s="2"/>
-      <c r="AJ82" s="2"/>
-      <c r="AK82" s="5"/>
-      <c r="AL82" s="5"/>
-      <c r="AM82" s="2"/>
-      <c r="AN82" s="2"/>
-      <c r="AO82" s="2"/>
-      <c r="AP82" s="2"/>
-      <c r="AQ82" s="2"/>
-      <c r="AR82" s="2"/>
-      <c r="AS82" s="2"/>
-      <c r="AT82" s="5"/>
-      <c r="AU82" s="5"/>
-      <c r="AV82" s="5"/>
-      <c r="AW82" s="5"/>
-      <c r="AX82" s="5"/>
-      <c r="AY82" s="5"/>
-      <c r="AZ82" s="5"/>
-      <c r="BA82" s="5"/>
-      <c r="BB82" s="4"/>
-    </row>
-    <row r="83" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
       <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
+      <c r="C83" s="4"/>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
-      <c r="J83" s="5"/>
+      <c r="I83" s="30"/>
+      <c r="J83" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
       <c r="M83" s="5"/>
@@ -4750,16 +4433,20 @@
       <c r="X83" s="5"/>
       <c r="Y83" s="5"/>
       <c r="Z83" s="4"/>
-      <c r="AC83" s="11"/>
+      <c r="AC83" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="AD83" s="5"/>
-      <c r="AE83" s="5"/>
+      <c r="AE83" s="4"/>
       <c r="AF83" s="5"/>
       <c r="AG83" s="5"/>
       <c r="AH83" s="5"/>
       <c r="AI83" s="5"/>
       <c r="AJ83" s="5"/>
-      <c r="AK83" s="5"/>
-      <c r="AL83" s="5"/>
+      <c r="AK83" s="30"/>
+      <c r="AL83" s="30" t="s">
+        <v>30</v>
+      </c>
       <c r="AM83" s="5"/>
       <c r="AN83" s="5"/>
       <c r="AO83" s="5"/>
@@ -4778,135 +4465,131 @@
       <c r="BB83" s="4"/>
     </row>
     <row r="84" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
-      <c r="B84" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="5"/>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5"/>
-      <c r="K84" s="5"/>
-      <c r="L84" s="5"/>
-      <c r="M84" s="5"/>
-      <c r="N84" s="5"/>
-      <c r="O84" s="5"/>
-      <c r="P84" s="5"/>
-      <c r="Q84" s="5"/>
-      <c r="R84" s="5"/>
-      <c r="S84" s="5"/>
-      <c r="T84" s="5"/>
-      <c r="U84" s="5"/>
-      <c r="V84" s="5"/>
-      <c r="W84" s="5"/>
-      <c r="X84" s="5"/>
-      <c r="Y84" s="5"/>
-      <c r="Z84" s="4"/>
-      <c r="AC84" s="11"/>
-      <c r="AD84" s="5"/>
-      <c r="AE84" s="5"/>
-      <c r="AF84" s="5"/>
-      <c r="AG84" s="5"/>
-      <c r="AH84" s="5"/>
-      <c r="AI84" s="5"/>
-      <c r="AJ84" s="5"/>
-      <c r="AK84" s="5"/>
-      <c r="AL84" s="5"/>
-      <c r="AM84" s="5"/>
-      <c r="AN84" s="5"/>
-      <c r="AO84" s="5"/>
-      <c r="AP84" s="5"/>
-      <c r="AQ84" s="5"/>
-      <c r="AR84" s="5"/>
-      <c r="AS84" s="5"/>
-      <c r="AT84" s="5"/>
-      <c r="AU84" s="5"/>
-      <c r="AV84" s="5"/>
-      <c r="AW84" s="5"/>
-      <c r="AX84" s="5"/>
-      <c r="AY84" s="5"/>
-      <c r="AZ84" s="5"/>
-      <c r="BA84" s="5"/>
-      <c r="BB84" s="4"/>
+      <c r="A84" s="3"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+      <c r="O84" s="2"/>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="2"/>
+      <c r="R84" s="2"/>
+      <c r="S84" s="2"/>
+      <c r="T84" s="2"/>
+      <c r="U84" s="2"/>
+      <c r="V84" s="2"/>
+      <c r="W84" s="2"/>
+      <c r="X84" s="2"/>
+      <c r="Y84" s="2"/>
+      <c r="Z84" s="1"/>
+      <c r="AC84" s="3"/>
+      <c r="AD84" s="2"/>
+      <c r="AE84" s="1"/>
+      <c r="AF84" s="2"/>
+      <c r="AG84" s="2"/>
+      <c r="AH84" s="2"/>
+      <c r="AI84" s="2"/>
+      <c r="AJ84" s="2"/>
+      <c r="AK84" s="2"/>
+      <c r="AL84" s="2"/>
+      <c r="AM84" s="2"/>
+      <c r="AN84" s="2"/>
+      <c r="AO84" s="2"/>
+      <c r="AP84" s="2"/>
+      <c r="AQ84" s="2"/>
+      <c r="AR84" s="2"/>
+      <c r="AS84" s="2"/>
+      <c r="AT84" s="2"/>
+      <c r="AU84" s="2"/>
+      <c r="AV84" s="2"/>
+      <c r="AW84" s="2"/>
+      <c r="AX84" s="2"/>
+      <c r="AY84" s="2"/>
+      <c r="AZ84" s="2"/>
+      <c r="BA84" s="2"/>
+      <c r="BB84" s="1"/>
     </row>
     <row r="85" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
-      <c r="O85" s="5"/>
-      <c r="P85" s="5"/>
-      <c r="Q85" s="5"/>
-      <c r="R85" s="5"/>
-      <c r="S85" s="5"/>
-      <c r="T85" s="5"/>
-      <c r="U85" s="5"/>
-      <c r="V85" s="5"/>
-      <c r="W85" s="5"/>
-      <c r="X85" s="5"/>
-      <c r="Y85" s="5"/>
-      <c r="Z85" s="4"/>
-      <c r="AC85" s="11"/>
-      <c r="AD85" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE85" s="5"/>
-      <c r="AF85" s="5"/>
-      <c r="AG85" s="5"/>
-      <c r="AH85" s="5"/>
-      <c r="AI85" s="5"/>
-      <c r="AJ85" s="5"/>
-      <c r="AK85" s="5"/>
-      <c r="AL85" s="5"/>
-      <c r="AM85" s="5"/>
-      <c r="AN85" s="5"/>
-      <c r="AO85" s="5"/>
-      <c r="AP85" s="5"/>
-      <c r="AQ85" s="5"/>
-      <c r="AR85" s="5"/>
-      <c r="AS85" s="5"/>
-      <c r="AT85" s="5"/>
-      <c r="AU85" s="5"/>
-      <c r="AV85" s="5"/>
-      <c r="AW85" s="5"/>
-      <c r="AX85" s="5"/>
-      <c r="AY85" s="5"/>
-      <c r="AZ85" s="5"/>
-      <c r="BA85" s="5"/>
-      <c r="BB85" s="4"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="8"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="8"/>
+      <c r="Q85" s="8"/>
+      <c r="R85" s="8"/>
+      <c r="S85" s="8"/>
+      <c r="T85" s="8"/>
+      <c r="U85" s="8"/>
+      <c r="V85" s="8"/>
+      <c r="W85" s="8"/>
+      <c r="X85" s="8"/>
+      <c r="Y85" s="8"/>
+      <c r="Z85" s="7"/>
+      <c r="AC85" s="9"/>
+      <c r="AD85" s="8"/>
+      <c r="AE85" s="8"/>
+      <c r="AF85" s="8"/>
+      <c r="AG85" s="8"/>
+      <c r="AH85" s="8"/>
+      <c r="AI85" s="8"/>
+      <c r="AJ85" s="8"/>
+      <c r="AK85" s="8"/>
+      <c r="AL85" s="8"/>
+      <c r="AM85" s="8"/>
+      <c r="AN85" s="8"/>
+      <c r="AO85" s="8"/>
+      <c r="AP85" s="8"/>
+      <c r="AQ85" s="8"/>
+      <c r="AR85" s="8"/>
+      <c r="AS85" s="8"/>
+      <c r="AT85" s="8"/>
+      <c r="AU85" s="8"/>
+      <c r="AV85" s="8"/>
+      <c r="AW85" s="8"/>
+      <c r="AX85" s="8"/>
+      <c r="AY85" s="8"/>
+      <c r="AZ85" s="8"/>
+      <c r="BA85" s="8"/>
+      <c r="BB85" s="7"/>
     </row>
     <row r="86" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
-      <c r="B86" s="23"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="23"/>
-      <c r="E86" s="23"/>
-      <c r="F86" s="23"/>
-      <c r="G86" s="23"/>
-      <c r="H86" s="23"/>
-      <c r="I86" s="23"/>
-      <c r="J86" s="23"/>
-      <c r="K86" s="23"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="23"/>
-      <c r="N86" s="23"/>
-      <c r="O86" s="5"/>
-      <c r="P86" s="5"/>
-      <c r="Q86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="5"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="8"/>
+      <c r="N86" s="8"/>
+      <c r="O86" s="8"/>
+      <c r="P86" s="8"/>
+      <c r="Q86" s="7"/>
       <c r="R86" s="5"/>
       <c r="S86" s="5"/>
       <c r="T86" s="5"/>
@@ -4917,22 +4600,22 @@
       <c r="Y86" s="5"/>
       <c r="Z86" s="4"/>
       <c r="AC86" s="11"/>
-      <c r="AD86" s="2"/>
-      <c r="AE86" s="2"/>
-      <c r="AF86" s="2"/>
-      <c r="AG86" s="2"/>
-      <c r="AH86" s="2"/>
-      <c r="AI86" s="2"/>
-      <c r="AJ86" s="2"/>
-      <c r="AK86" s="2"/>
-      <c r="AL86" s="2"/>
-      <c r="AM86" s="2"/>
-      <c r="AN86" s="2"/>
-      <c r="AO86" s="2"/>
-      <c r="AP86" s="2"/>
-      <c r="AQ86" s="5"/>
-      <c r="AR86" s="5"/>
-      <c r="AS86" s="5"/>
+      <c r="AD86" s="5"/>
+      <c r="AE86" s="5"/>
+      <c r="AF86" s="5"/>
+      <c r="AG86" s="5"/>
+      <c r="AH86" s="5"/>
+      <c r="AI86" s="5"/>
+      <c r="AJ86" s="5"/>
+      <c r="AK86" s="5"/>
+      <c r="AL86" s="5"/>
+      <c r="AM86" s="5"/>
+      <c r="AN86" s="9"/>
+      <c r="AO86" s="8"/>
+      <c r="AP86" s="8"/>
+      <c r="AQ86" s="8"/>
+      <c r="AR86" s="8"/>
+      <c r="AS86" s="7"/>
       <c r="AT86" s="5"/>
       <c r="AU86" s="5"/>
       <c r="AV86" s="5"/>
@@ -4945,22 +4628,22 @@
     </row>
     <row r="87" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>
-      <c r="B87" s="23"/>
-      <c r="C87" s="23"/>
-      <c r="D87" s="23"/>
-      <c r="E87" s="23"/>
-      <c r="F87" s="23"/>
-      <c r="G87" s="23"/>
-      <c r="H87" s="23"/>
-      <c r="I87" s="23"/>
-      <c r="J87" s="23"/>
-      <c r="K87" s="23"/>
-      <c r="L87" s="23"/>
-      <c r="M87" s="23"/>
-      <c r="N87" s="23"/>
+      <c r="B87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="5"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="11"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
       <c r="O87" s="5"/>
       <c r="P87" s="5"/>
-      <c r="Q87" s="5"/>
+      <c r="Q87" s="4"/>
       <c r="R87" s="5"/>
       <c r="S87" s="5"/>
       <c r="T87" s="5"/>
@@ -4981,12 +4664,12 @@
       <c r="AK87" s="5"/>
       <c r="AL87" s="5"/>
       <c r="AM87" s="5"/>
-      <c r="AN87" s="5"/>
+      <c r="AN87" s="11"/>
       <c r="AO87" s="5"/>
       <c r="AP87" s="5"/>
       <c r="AQ87" s="5"/>
       <c r="AR87" s="5"/>
-      <c r="AS87" s="5"/>
+      <c r="AS87" s="4"/>
       <c r="AT87" s="5"/>
       <c r="AU87" s="5"/>
       <c r="AV87" s="5"/>
@@ -5009,12 +4692,14 @@
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
       <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
+      <c r="L88" s="11"/>
       <c r="M88" s="5"/>
-      <c r="N88" s="5"/>
+      <c r="N88" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="O88" s="5"/>
       <c r="P88" s="5"/>
-      <c r="Q88" s="5"/>
+      <c r="Q88" s="4"/>
       <c r="R88" s="5"/>
       <c r="S88" s="5"/>
       <c r="T88" s="5"/>
@@ -5025,9 +4710,7 @@
       <c r="Y88" s="5"/>
       <c r="Z88" s="4"/>
       <c r="AC88" s="11"/>
-      <c r="AD88" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="AD88" s="5"/>
       <c r="AE88" s="5"/>
       <c r="AF88" s="5"/>
       <c r="AG88" s="5"/>
@@ -5037,12 +4720,14 @@
       <c r="AK88" s="5"/>
       <c r="AL88" s="5"/>
       <c r="AM88" s="5"/>
-      <c r="AN88" s="5"/>
+      <c r="AN88" s="11"/>
       <c r="AO88" s="5"/>
-      <c r="AP88" s="5"/>
+      <c r="AP88" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="AQ88" s="5"/>
       <c r="AR88" s="5"/>
-      <c r="AS88" s="5"/>
+      <c r="AS88" s="4"/>
       <c r="AT88" s="5"/>
       <c r="AU88" s="5"/>
       <c r="AV88" s="5"/>
@@ -5055,9 +4740,7 @@
     </row>
     <row r="89" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A89" s="11"/>
-      <c r="B89" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
       <c r="E89" s="5"/>
@@ -5067,12 +4750,12 @@
       <c r="I89" s="5"/>
       <c r="J89" s="5"/>
       <c r="K89" s="5"/>
-      <c r="L89" s="5"/>
+      <c r="L89" s="11"/>
       <c r="M89" s="5"/>
       <c r="N89" s="5"/>
       <c r="O89" s="5"/>
       <c r="P89" s="5"/>
-      <c r="Q89" s="5"/>
+      <c r="Q89" s="4"/>
       <c r="R89" s="5"/>
       <c r="S89" s="5"/>
       <c r="T89" s="5"/>
@@ -5083,22 +4766,22 @@
       <c r="Y89" s="5"/>
       <c r="Z89" s="4"/>
       <c r="AC89" s="11"/>
-      <c r="AD89" s="2"/>
-      <c r="AE89" s="2"/>
-      <c r="AF89" s="2"/>
-      <c r="AG89" s="2"/>
-      <c r="AH89" s="2"/>
-      <c r="AI89" s="2"/>
-      <c r="AJ89" s="2"/>
-      <c r="AK89" s="2"/>
-      <c r="AL89" s="2"/>
-      <c r="AM89" s="2"/>
-      <c r="AN89" s="2"/>
-      <c r="AO89" s="2"/>
-      <c r="AP89" s="2"/>
+      <c r="AD89" s="5"/>
+      <c r="AE89" s="5"/>
+      <c r="AF89" s="5"/>
+      <c r="AG89" s="5"/>
+      <c r="AH89" s="5"/>
+      <c r="AI89" s="5"/>
+      <c r="AJ89" s="5"/>
+      <c r="AK89" s="5"/>
+      <c r="AL89" s="5"/>
+      <c r="AM89" s="5"/>
+      <c r="AN89" s="11"/>
+      <c r="AO89" s="5"/>
+      <c r="AP89" s="5"/>
       <c r="AQ89" s="5"/>
       <c r="AR89" s="5"/>
-      <c r="AS89" s="5"/>
+      <c r="AS89" s="4"/>
       <c r="AT89" s="5"/>
       <c r="AU89" s="5"/>
       <c r="AV89" s="5"/>
@@ -5111,22 +4794,22 @@
     </row>
     <row r="90" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A90" s="11"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
+      <c r="B90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
       <c r="J90" s="5"/>
       <c r="K90" s="5"/>
-      <c r="L90" s="5"/>
+      <c r="L90" s="11"/>
       <c r="M90" s="5"/>
       <c r="N90" s="5"/>
       <c r="O90" s="5"/>
       <c r="P90" s="5"/>
-      <c r="Q90" s="5"/>
+      <c r="Q90" s="4"/>
       <c r="R90" s="5"/>
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
@@ -5137,22 +4820,22 @@
       <c r="Y90" s="5"/>
       <c r="Z90" s="4"/>
       <c r="AC90" s="11"/>
-      <c r="AD90" s="23"/>
-      <c r="AE90" s="23"/>
-      <c r="AF90" s="23"/>
-      <c r="AG90" s="23"/>
-      <c r="AH90" s="23"/>
-      <c r="AI90" s="23"/>
-      <c r="AJ90" s="23"/>
-      <c r="AK90" s="23"/>
-      <c r="AL90" s="23"/>
-      <c r="AM90" s="23"/>
-      <c r="AN90" s="23"/>
-      <c r="AO90" s="23"/>
-      <c r="AP90" s="23"/>
+      <c r="AD90" s="5"/>
+      <c r="AE90" s="5"/>
+      <c r="AF90" s="5"/>
+      <c r="AG90" s="5"/>
+      <c r="AH90" s="5"/>
+      <c r="AI90" s="5"/>
+      <c r="AJ90" s="5"/>
+      <c r="AK90" s="5"/>
+      <c r="AL90" s="5"/>
+      <c r="AM90" s="5"/>
+      <c r="AN90" s="11"/>
+      <c r="AO90" s="5"/>
+      <c r="AP90" s="5"/>
       <c r="AQ90" s="5"/>
       <c r="AR90" s="5"/>
-      <c r="AS90" s="5"/>
+      <c r="AS90" s="4"/>
       <c r="AT90" s="5"/>
       <c r="AU90" s="5"/>
       <c r="AV90" s="5"/>
@@ -5175,12 +4858,12 @@
       <c r="I91" s="5"/>
       <c r="J91" s="5"/>
       <c r="K91" s="5"/>
-      <c r="L91" s="5"/>
-      <c r="M91" s="5"/>
-      <c r="N91" s="5"/>
-      <c r="O91" s="5"/>
-      <c r="P91" s="5"/>
-      <c r="Q91" s="5"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="2"/>
+      <c r="N91" s="2"/>
+      <c r="O91" s="2"/>
+      <c r="P91" s="2"/>
+      <c r="Q91" s="1"/>
       <c r="R91" s="5"/>
       <c r="S91" s="5"/>
       <c r="T91" s="5"/>
@@ -5191,22 +4874,22 @@
       <c r="Y91" s="5"/>
       <c r="Z91" s="4"/>
       <c r="AC91" s="11"/>
-      <c r="AD91" s="23"/>
-      <c r="AE91" s="23"/>
-      <c r="AF91" s="23"/>
-      <c r="AG91" s="23"/>
-      <c r="AH91" s="23"/>
-      <c r="AI91" s="23"/>
-      <c r="AJ91" s="23"/>
-      <c r="AK91" s="23"/>
-      <c r="AL91" s="23"/>
-      <c r="AM91" s="23"/>
-      <c r="AN91" s="23"/>
-      <c r="AO91" s="23"/>
-      <c r="AP91" s="23"/>
-      <c r="AQ91" s="5"/>
-      <c r="AR91" s="5"/>
-      <c r="AS91" s="5"/>
+      <c r="AD91" s="5"/>
+      <c r="AE91" s="5"/>
+      <c r="AF91" s="5"/>
+      <c r="AG91" s="5"/>
+      <c r="AH91" s="5"/>
+      <c r="AI91" s="5"/>
+      <c r="AJ91" s="5"/>
+      <c r="AK91" s="5"/>
+      <c r="AL91" s="5"/>
+      <c r="AM91" s="5"/>
+      <c r="AN91" s="3"/>
+      <c r="AO91" s="2"/>
+      <c r="AP91" s="2"/>
+      <c r="AQ91" s="2"/>
+      <c r="AR91" s="2"/>
+      <c r="AS91" s="1"/>
       <c r="AT91" s="5"/>
       <c r="AU91" s="5"/>
       <c r="AV91" s="5"/>
@@ -5219,17 +4902,13 @@
     </row>
     <row r="92" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A92" s="11"/>
-      <c r="B92" s="30" t="s">
-        <v>34</v>
-      </c>
+      <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
       <c r="E92" s="5"/>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
-      <c r="H92" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="H92" s="5"/>
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
       <c r="K92" s="5"/>
@@ -5277,28 +4956,26 @@
     </row>
     <row r="93" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A93" s="11"/>
-      <c r="B93" s="22"/>
-      <c r="C93" s="23"/>
-      <c r="D93" s="23"/>
-      <c r="E93" s="24" t="s">
-        <v>8</v>
-      </c>
+      <c r="B93" s="5"/>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
-      <c r="H93" s="22"/>
-      <c r="I93" s="23"/>
-      <c r="J93" s="23"/>
-      <c r="K93" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="L93" s="5"/>
-      <c r="M93" s="5"/>
-      <c r="N93" s="5"/>
-      <c r="O93" s="5"/>
-      <c r="P93" s="5"/>
-      <c r="Q93" s="5"/>
-      <c r="R93" s="5"/>
-      <c r="S93" s="5"/>
+      <c r="H93" s="5"/>
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+      <c r="K93" s="5"/>
+      <c r="L93" s="22"/>
+      <c r="M93" s="23"/>
+      <c r="N93" s="23"/>
+      <c r="O93" s="23"/>
+      <c r="P93" s="24"/>
+      <c r="Q93" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="R93" s="23"/>
+      <c r="S93" s="24"/>
       <c r="T93" s="5"/>
       <c r="U93" s="5"/>
       <c r="V93" s="5"/>
@@ -5307,9 +4984,7 @@
       <c r="Y93" s="5"/>
       <c r="Z93" s="4"/>
       <c r="AC93" s="11"/>
-      <c r="AD93" s="5" t="s">
-        <v>35</v>
-      </c>
+      <c r="AD93" s="5"/>
       <c r="AE93" s="5"/>
       <c r="AF93" s="5"/>
       <c r="AG93" s="5"/>
@@ -5319,14 +4994,16 @@
       <c r="AK93" s="5"/>
       <c r="AL93" s="5"/>
       <c r="AM93" s="5"/>
-      <c r="AN93" s="5"/>
-      <c r="AO93" s="5"/>
-      <c r="AP93" s="5"/>
-      <c r="AQ93" s="5"/>
-      <c r="AR93" s="5"/>
-      <c r="AS93" s="5"/>
-      <c r="AT93" s="5"/>
-      <c r="AU93" s="5"/>
+      <c r="AN93" s="22"/>
+      <c r="AO93" s="23"/>
+      <c r="AP93" s="23"/>
+      <c r="AQ93" s="23"/>
+      <c r="AR93" s="24"/>
+      <c r="AS93" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="AT93" s="23"/>
+      <c r="AU93" s="24"/>
       <c r="AV93" s="5"/>
       <c r="AW93" s="5"/>
       <c r="AX93" s="5"/>
@@ -5363,11 +5040,11 @@
       <c r="Y94" s="5"/>
       <c r="Z94" s="4"/>
       <c r="AC94" s="11"/>
-      <c r="AD94" s="2"/>
-      <c r="AE94" s="2"/>
-      <c r="AF94" s="2"/>
-      <c r="AG94" s="2"/>
-      <c r="AH94" s="2"/>
+      <c r="AD94" s="5"/>
+      <c r="AE94" s="5"/>
+      <c r="AF94" s="5"/>
+      <c r="AG94" s="5"/>
+      <c r="AH94" s="5"/>
       <c r="AI94" s="5"/>
       <c r="AJ94" s="5"/>
       <c r="AK94" s="5"/>
@@ -5392,7 +5069,7 @@
     <row r="95" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A95" s="11"/>
       <c r="B95" s="5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -5402,7 +5079,9 @@
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
-      <c r="K95" s="5"/>
+      <c r="K95" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="L95" s="5"/>
       <c r="M95" s="5"/>
       <c r="N95" s="5"/>
@@ -5419,7 +5098,9 @@
       <c r="Y95" s="5"/>
       <c r="Z95" s="4"/>
       <c r="AC95" s="11"/>
-      <c r="AD95" s="5"/>
+      <c r="AD95" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="AE95" s="5"/>
       <c r="AF95" s="5"/>
       <c r="AG95" s="5"/>
@@ -5428,7 +5109,9 @@
       <c r="AJ95" s="5"/>
       <c r="AK95" s="5"/>
       <c r="AL95" s="5"/>
-      <c r="AM95" s="5"/>
+      <c r="AM95" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="AN95" s="5"/>
       <c r="AO95" s="5"/>
       <c r="AP95" s="5"/>
@@ -5453,16 +5136,16 @@
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="5"/>
+      <c r="H96" s="2"/>
       <c r="I96" s="5"/>
       <c r="J96" s="5"/>
-      <c r="K96" s="5"/>
-      <c r="L96" s="5"/>
-      <c r="M96" s="5"/>
-      <c r="N96" s="5"/>
-      <c r="O96" s="5"/>
-      <c r="P96" s="5"/>
-      <c r="Q96" s="5"/>
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
+      <c r="N96" s="2"/>
+      <c r="O96" s="2"/>
+      <c r="P96" s="2"/>
+      <c r="Q96" s="2"/>
       <c r="R96" s="5"/>
       <c r="S96" s="5"/>
       <c r="T96" s="5"/>
@@ -5473,26 +5156,22 @@
       <c r="Y96" s="5"/>
       <c r="Z96" s="4"/>
       <c r="AC96" s="11"/>
-      <c r="AD96" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE96" s="5"/>
-      <c r="AF96" s="5"/>
-      <c r="AG96" s="5"/>
-      <c r="AH96" s="5"/>
-      <c r="AI96" s="5"/>
-      <c r="AJ96" s="30" t="s">
-        <v>12</v>
-      </c>
+      <c r="AD96" s="2"/>
+      <c r="AE96" s="2"/>
+      <c r="AF96" s="2"/>
+      <c r="AG96" s="2"/>
+      <c r="AH96" s="2"/>
+      <c r="AI96" s="2"/>
+      <c r="AJ96" s="2"/>
       <c r="AK96" s="5"/>
       <c r="AL96" s="5"/>
-      <c r="AM96" s="5"/>
-      <c r="AN96" s="5"/>
-      <c r="AO96" s="5"/>
-      <c r="AP96" s="5"/>
-      <c r="AQ96" s="5"/>
-      <c r="AR96" s="5"/>
-      <c r="AS96" s="5"/>
+      <c r="AM96" s="2"/>
+      <c r="AN96" s="2"/>
+      <c r="AO96" s="2"/>
+      <c r="AP96" s="2"/>
+      <c r="AQ96" s="2"/>
+      <c r="AR96" s="2"/>
+      <c r="AS96" s="2"/>
       <c r="AT96" s="5"/>
       <c r="AU96" s="5"/>
       <c r="AV96" s="5"/>
@@ -5531,20 +5210,16 @@
       <c r="Y97" s="5"/>
       <c r="Z97" s="4"/>
       <c r="AC97" s="11"/>
-      <c r="AD97" s="22"/>
-      <c r="AE97" s="23"/>
-      <c r="AF97" s="23"/>
-      <c r="AG97" s="24" t="s">
-        <v>8</v>
-      </c>
+      <c r="AD97" s="5"/>
+      <c r="AE97" s="5"/>
+      <c r="AF97" s="5"/>
+      <c r="AG97" s="5"/>
       <c r="AH97" s="5"/>
       <c r="AI97" s="5"/>
-      <c r="AJ97" s="22"/>
-      <c r="AK97" s="23"/>
-      <c r="AL97" s="23"/>
-      <c r="AM97" s="24" t="s">
-        <v>8</v>
-      </c>
+      <c r="AJ97" s="5"/>
+      <c r="AK97" s="5"/>
+      <c r="AL97" s="5"/>
+      <c r="AM97" s="5"/>
       <c r="AN97" s="5"/>
       <c r="AO97" s="5"/>
       <c r="AP97" s="5"/>
@@ -5563,12 +5238,12 @@
     </row>
     <row r="98" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A98" s="11"/>
-      <c r="B98" s="5"/>
+      <c r="B98" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C98" s="5"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="5" t="s">
-        <v>37</v>
-      </c>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
       <c r="F98" s="5"/>
       <c r="G98" s="5"/>
       <c r="H98" s="5"/>
@@ -5619,19 +5294,19 @@
     </row>
     <row r="99" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A99" s="11"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="5"/>
-      <c r="J99" s="5"/>
-      <c r="K99" s="5"/>
-      <c r="L99" s="5"/>
-      <c r="M99" s="5"/>
-      <c r="N99" s="5"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
+      <c r="L99" s="2"/>
+      <c r="M99" s="2"/>
+      <c r="N99" s="2"/>
       <c r="O99" s="5"/>
       <c r="P99" s="5"/>
       <c r="Q99" s="5"/>
@@ -5646,7 +5321,7 @@
       <c r="Z99" s="4"/>
       <c r="AC99" s="11"/>
       <c r="AD99" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="AE99" s="5"/>
       <c r="AF99" s="5"/>
@@ -5675,21 +5350,19 @@
     </row>
     <row r="100" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A100" s="11"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F100" s="33"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23"/>
+      <c r="D100" s="23"/>
+      <c r="E100" s="23"/>
+      <c r="F100" s="23"/>
       <c r="G100" s="23"/>
       <c r="H100" s="23"/>
-      <c r="I100" s="24"/>
-      <c r="J100" s="5"/>
-      <c r="K100" s="5"/>
-      <c r="L100" s="5"/>
-      <c r="M100" s="5"/>
-      <c r="N100" s="5"/>
+      <c r="I100" s="23"/>
+      <c r="J100" s="23"/>
+      <c r="K100" s="23"/>
+      <c r="L100" s="23"/>
+      <c r="M100" s="23"/>
+      <c r="N100" s="23"/>
       <c r="O100" s="5"/>
       <c r="P100" s="5"/>
       <c r="Q100" s="5"/>
@@ -5709,13 +5382,13 @@
       <c r="AG100" s="2"/>
       <c r="AH100" s="2"/>
       <c r="AI100" s="2"/>
-      <c r="AJ100" s="5"/>
-      <c r="AK100" s="5"/>
-      <c r="AL100" s="5"/>
-      <c r="AM100" s="5"/>
-      <c r="AN100" s="5"/>
-      <c r="AO100" s="5"/>
-      <c r="AP100" s="5"/>
+      <c r="AJ100" s="2"/>
+      <c r="AK100" s="2"/>
+      <c r="AL100" s="2"/>
+      <c r="AM100" s="2"/>
+      <c r="AN100" s="2"/>
+      <c r="AO100" s="2"/>
+      <c r="AP100" s="2"/>
       <c r="AQ100" s="5"/>
       <c r="AR100" s="5"/>
       <c r="AS100" s="5"/>
@@ -5731,19 +5404,19 @@
     </row>
     <row r="101" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A101" s="11"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
-      <c r="J101" s="5"/>
-      <c r="K101" s="5"/>
-      <c r="L101" s="5"/>
-      <c r="M101" s="5"/>
-      <c r="N101" s="5"/>
+      <c r="B101" s="23"/>
+      <c r="C101" s="23"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="23"/>
+      <c r="G101" s="23"/>
+      <c r="H101" s="23"/>
+      <c r="I101" s="23"/>
+      <c r="J101" s="23"/>
+      <c r="K101" s="23"/>
+      <c r="L101" s="23"/>
+      <c r="M101" s="23"/>
+      <c r="N101" s="23"/>
       <c r="O101" s="5"/>
       <c r="P101" s="5"/>
       <c r="Q101" s="5"/>
@@ -5811,7 +5484,9 @@
       <c r="Y102" s="5"/>
       <c r="Z102" s="4"/>
       <c r="AC102" s="11"/>
-      <c r="AD102" s="5"/>
+      <c r="AD102" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="AE102" s="5"/>
       <c r="AF102" s="5"/>
       <c r="AG102" s="5"/>
@@ -5838,48 +5513,48 @@
       <c r="BB102" s="4"/>
     </row>
     <row r="103" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A103" s="3"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-      <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
-      <c r="L103" s="2"/>
-      <c r="M103" s="2"/>
-      <c r="N103" s="2"/>
-      <c r="O103" s="2"/>
-      <c r="P103" s="2"/>
-      <c r="Q103" s="2"/>
-      <c r="R103" s="2"/>
-      <c r="S103" s="2"/>
-      <c r="T103" s="2"/>
-      <c r="U103" s="2"/>
-      <c r="V103" s="2"/>
-      <c r="W103" s="2"/>
-      <c r="X103" s="2"/>
-      <c r="Y103" s="2"/>
-      <c r="Z103" s="1"/>
+      <c r="A103" s="11"/>
+      <c r="B103" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="5"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+      <c r="K103" s="5"/>
+      <c r="L103" s="5"/>
+      <c r="M103" s="5"/>
+      <c r="N103" s="5"/>
+      <c r="O103" s="5"/>
+      <c r="P103" s="5"/>
+      <c r="Q103" s="5"/>
+      <c r="R103" s="5"/>
+      <c r="S103" s="5"/>
+      <c r="T103" s="5"/>
+      <c r="U103" s="5"/>
+      <c r="V103" s="5"/>
+      <c r="W103" s="5"/>
+      <c r="X103" s="5"/>
+      <c r="Y103" s="5"/>
+      <c r="Z103" s="4"/>
       <c r="AC103" s="11"/>
-      <c r="AD103" s="28"/>
-      <c r="AE103" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="AD103" s="2"/>
+      <c r="AE103" s="2"/>
       <c r="AF103" s="2"/>
       <c r="AG103" s="2"/>
       <c r="AH103" s="2"/>
       <c r="AI103" s="2"/>
       <c r="AJ103" s="2"/>
       <c r="AK103" s="2"/>
-      <c r="AL103" s="5"/>
-      <c r="AM103" s="5"/>
-      <c r="AN103" s="5"/>
-      <c r="AO103" s="5"/>
-      <c r="AP103" s="5"/>
+      <c r="AL103" s="2"/>
+      <c r="AM103" s="2"/>
+      <c r="AN103" s="2"/>
+      <c r="AO103" s="2"/>
+      <c r="AP103" s="2"/>
       <c r="AQ103" s="5"/>
       <c r="AR103" s="5"/>
       <c r="AS103" s="5"/>
@@ -5894,20 +5569,46 @@
       <c r="BB103" s="4"/>
     </row>
     <row r="104" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A104" s="11"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="5"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="5"/>
+      <c r="K104" s="5"/>
+      <c r="L104" s="5"/>
+      <c r="M104" s="5"/>
+      <c r="N104" s="5"/>
+      <c r="O104" s="5"/>
+      <c r="P104" s="5"/>
+      <c r="Q104" s="5"/>
+      <c r="R104" s="5"/>
+      <c r="S104" s="5"/>
+      <c r="T104" s="5"/>
+      <c r="U104" s="5"/>
+      <c r="V104" s="5"/>
+      <c r="W104" s="5"/>
+      <c r="X104" s="5"/>
+      <c r="Y104" s="5"/>
+      <c r="Z104" s="4"/>
       <c r="AC104" s="11"/>
-      <c r="AD104" s="5"/>
-      <c r="AE104" s="5"/>
-      <c r="AF104" s="5"/>
-      <c r="AG104" s="5"/>
-      <c r="AH104" s="5"/>
-      <c r="AI104" s="5"/>
-      <c r="AJ104" s="5"/>
-      <c r="AK104" s="5"/>
-      <c r="AL104" s="5"/>
-      <c r="AM104" s="5"/>
-      <c r="AN104" s="5"/>
-      <c r="AO104" s="5"/>
-      <c r="AP104" s="5"/>
+      <c r="AD104" s="23"/>
+      <c r="AE104" s="23"/>
+      <c r="AF104" s="23"/>
+      <c r="AG104" s="23"/>
+      <c r="AH104" s="23"/>
+      <c r="AI104" s="23"/>
+      <c r="AJ104" s="23"/>
+      <c r="AK104" s="23"/>
+      <c r="AL104" s="23"/>
+      <c r="AM104" s="23"/>
+      <c r="AN104" s="23"/>
+      <c r="AO104" s="23"/>
+      <c r="AP104" s="23"/>
       <c r="AQ104" s="5"/>
       <c r="AR104" s="5"/>
       <c r="AS104" s="5"/>
@@ -5922,22 +5623,46 @@
       <c r="BB104" s="4"/>
     </row>
     <row r="105" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A105" s="11"/>
+      <c r="B105" s="5"/>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
+      <c r="J105" s="5"/>
+      <c r="K105" s="5"/>
+      <c r="L105" s="5"/>
+      <c r="M105" s="5"/>
+      <c r="N105" s="5"/>
+      <c r="O105" s="5"/>
+      <c r="P105" s="5"/>
+      <c r="Q105" s="5"/>
+      <c r="R105" s="5"/>
+      <c r="S105" s="5"/>
+      <c r="T105" s="5"/>
+      <c r="U105" s="5"/>
+      <c r="V105" s="5"/>
+      <c r="W105" s="5"/>
+      <c r="X105" s="5"/>
+      <c r="Y105" s="5"/>
+      <c r="Z105" s="4"/>
       <c r="AC105" s="11"/>
-      <c r="AD105" s="28"/>
-      <c r="AE105" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF105" s="2"/>
-      <c r="AG105" s="2"/>
-      <c r="AH105" s="2"/>
-      <c r="AI105" s="2"/>
-      <c r="AJ105" s="2"/>
-      <c r="AK105" s="2"/>
-      <c r="AL105" s="5"/>
-      <c r="AM105" s="5"/>
-      <c r="AN105" s="5"/>
-      <c r="AO105" s="5"/>
-      <c r="AP105" s="5"/>
+      <c r="AD105" s="23"/>
+      <c r="AE105" s="23"/>
+      <c r="AF105" s="23"/>
+      <c r="AG105" s="23"/>
+      <c r="AH105" s="23"/>
+      <c r="AI105" s="23"/>
+      <c r="AJ105" s="23"/>
+      <c r="AK105" s="23"/>
+      <c r="AL105" s="23"/>
+      <c r="AM105" s="23"/>
+      <c r="AN105" s="23"/>
+      <c r="AO105" s="23"/>
+      <c r="AP105" s="23"/>
       <c r="AQ105" s="5"/>
       <c r="AR105" s="5"/>
       <c r="AS105" s="5"/>
@@ -5952,6 +5677,36 @@
       <c r="BB105" s="4"/>
     </row>
     <row r="106" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A106" s="11"/>
+      <c r="B106" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="5"/>
+      <c r="H106" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+      <c r="L106" s="5"/>
+      <c r="M106" s="5"/>
+      <c r="N106" s="5"/>
+      <c r="O106" s="5"/>
+      <c r="P106" s="5"/>
+      <c r="Q106" s="5"/>
+      <c r="R106" s="5"/>
+      <c r="S106" s="5"/>
+      <c r="T106" s="5"/>
+      <c r="U106" s="5"/>
+      <c r="V106" s="5"/>
+      <c r="W106" s="5"/>
+      <c r="X106" s="5"/>
+      <c r="Y106" s="5"/>
+      <c r="Z106" s="4"/>
       <c r="AC106" s="11"/>
       <c r="AD106" s="5"/>
       <c r="AE106" s="5"/>
@@ -5980,20 +5735,47 @@
       <c r="BB106" s="4"/>
     </row>
     <row r="107" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="F107" t="s">
-        <v>43</v>
-      </c>
+      <c r="A107" s="11"/>
+      <c r="B107" s="22"/>
+      <c r="C107" s="23"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
+      <c r="H107" s="22"/>
+      <c r="I107" s="23"/>
+      <c r="J107" s="23"/>
+      <c r="K107" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="L107" s="5"/>
+      <c r="M107" s="5"/>
+      <c r="N107" s="5"/>
+      <c r="O107" s="5"/>
+      <c r="P107" s="5"/>
+      <c r="Q107" s="5"/>
+      <c r="R107" s="5"/>
+      <c r="S107" s="5"/>
+      <c r="T107" s="5"/>
+      <c r="U107" s="5"/>
+      <c r="V107" s="5"/>
+      <c r="W107" s="5"/>
+      <c r="X107" s="5"/>
+      <c r="Y107" s="5"/>
+      <c r="Z107" s="4"/>
       <c r="AC107" s="11"/>
-      <c r="AD107" s="28"/>
-      <c r="AE107" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF107" s="2"/>
-      <c r="AG107" s="2"/>
-      <c r="AH107" s="2"/>
-      <c r="AI107" s="2"/>
-      <c r="AJ107" s="2"/>
-      <c r="AK107" s="2"/>
+      <c r="AD107" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AE107" s="5"/>
+      <c r="AF107" s="5"/>
+      <c r="AG107" s="5"/>
+      <c r="AH107" s="5"/>
+      <c r="AI107" s="5"/>
+      <c r="AJ107" s="5"/>
+      <c r="AK107" s="5"/>
       <c r="AL107" s="5"/>
       <c r="AM107" s="5"/>
       <c r="AN107" s="5"/>
@@ -6013,12 +5795,38 @@
       <c r="BB107" s="4"/>
     </row>
     <row r="108" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A108" s="11"/>
+      <c r="B108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="5"/>
+      <c r="G108" s="5"/>
+      <c r="H108" s="5"/>
+      <c r="I108" s="5"/>
+      <c r="J108" s="5"/>
+      <c r="K108" s="5"/>
+      <c r="L108" s="5"/>
+      <c r="M108" s="5"/>
+      <c r="N108" s="5"/>
+      <c r="O108" s="5"/>
+      <c r="P108" s="5"/>
+      <c r="Q108" s="5"/>
+      <c r="R108" s="5"/>
+      <c r="S108" s="5"/>
+      <c r="T108" s="5"/>
+      <c r="U108" s="5"/>
+      <c r="V108" s="5"/>
+      <c r="W108" s="5"/>
+      <c r="X108" s="5"/>
+      <c r="Y108" s="5"/>
+      <c r="Z108" s="4"/>
       <c r="AC108" s="11"/>
-      <c r="AD108" s="5"/>
-      <c r="AE108" s="5"/>
-      <c r="AF108" s="5"/>
-      <c r="AG108" s="5"/>
-      <c r="AH108" s="5"/>
+      <c r="AD108" s="2"/>
+      <c r="AE108" s="2"/>
+      <c r="AF108" s="2"/>
+      <c r="AG108" s="2"/>
+      <c r="AH108" s="2"/>
       <c r="AI108" s="5"/>
       <c r="AJ108" s="5"/>
       <c r="AK108" s="5"/>
@@ -6041,17 +5849,43 @@
       <c r="BB108" s="4"/>
     </row>
     <row r="109" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A109" s="11"/>
+      <c r="B109" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="5"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="5"/>
+      <c r="L109" s="5"/>
+      <c r="M109" s="5"/>
+      <c r="N109" s="5"/>
+      <c r="O109" s="5"/>
+      <c r="P109" s="5"/>
+      <c r="Q109" s="5"/>
+      <c r="R109" s="5"/>
+      <c r="S109" s="5"/>
+      <c r="T109" s="5"/>
+      <c r="U109" s="5"/>
+      <c r="V109" s="5"/>
+      <c r="W109" s="5"/>
+      <c r="X109" s="5"/>
+      <c r="Y109" s="5"/>
+      <c r="Z109" s="4"/>
       <c r="AC109" s="11"/>
-      <c r="AD109" s="28"/>
-      <c r="AE109" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AF109" s="2"/>
-      <c r="AG109" s="2"/>
-      <c r="AH109" s="2"/>
-      <c r="AI109" s="2"/>
-      <c r="AJ109" s="2"/>
-      <c r="AK109" s="2"/>
+      <c r="AD109" s="5"/>
+      <c r="AE109" s="5"/>
+      <c r="AF109" s="5"/>
+      <c r="AG109" s="5"/>
+      <c r="AH109" s="5"/>
+      <c r="AI109" s="5"/>
+      <c r="AJ109" s="5"/>
+      <c r="AK109" s="5"/>
       <c r="AL109" s="5"/>
       <c r="AM109" s="5"/>
       <c r="AN109" s="5"/>
@@ -6071,14 +5905,44 @@
       <c r="BB109" s="4"/>
     </row>
     <row r="110" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A110" s="11"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+      <c r="H110" s="5"/>
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="5"/>
+      <c r="L110" s="5"/>
+      <c r="M110" s="5"/>
+      <c r="N110" s="5"/>
+      <c r="O110" s="5"/>
+      <c r="P110" s="5"/>
+      <c r="Q110" s="5"/>
+      <c r="R110" s="5"/>
+      <c r="S110" s="5"/>
+      <c r="T110" s="5"/>
+      <c r="U110" s="5"/>
+      <c r="V110" s="5"/>
+      <c r="W110" s="5"/>
+      <c r="X110" s="5"/>
+      <c r="Y110" s="5"/>
+      <c r="Z110" s="4"/>
       <c r="AC110" s="11"/>
-      <c r="AD110" s="5"/>
+      <c r="AD110" s="30" t="s">
+        <v>34</v>
+      </c>
       <c r="AE110" s="5"/>
       <c r="AF110" s="5"/>
       <c r="AG110" s="5"/>
       <c r="AH110" s="5"/>
       <c r="AI110" s="5"/>
-      <c r="AJ110" s="5"/>
+      <c r="AJ110" s="30" t="s">
+        <v>12</v>
+      </c>
       <c r="AK110" s="5"/>
       <c r="AL110" s="5"/>
       <c r="AM110" s="5"/>
@@ -6099,17 +5963,47 @@
       <c r="BB110" s="4"/>
     </row>
     <row r="111" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A111" s="11"/>
+      <c r="B111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="5"/>
+      <c r="G111" s="5"/>
+      <c r="H111" s="5"/>
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="5"/>
+      <c r="M111" s="5"/>
+      <c r="N111" s="5"/>
+      <c r="O111" s="5"/>
+      <c r="P111" s="5"/>
+      <c r="Q111" s="5"/>
+      <c r="R111" s="5"/>
+      <c r="S111" s="5"/>
+      <c r="T111" s="5"/>
+      <c r="U111" s="5"/>
+      <c r="V111" s="5"/>
+      <c r="W111" s="5"/>
+      <c r="X111" s="5"/>
+      <c r="Y111" s="5"/>
+      <c r="Z111" s="4"/>
       <c r="AC111" s="11"/>
-      <c r="AD111" s="5"/>
-      <c r="AE111" s="5"/>
-      <c r="AF111" s="5"/>
-      <c r="AG111" s="5"/>
+      <c r="AD111" s="22"/>
+      <c r="AE111" s="23"/>
+      <c r="AF111" s="23"/>
+      <c r="AG111" s="24" t="s">
+        <v>8</v>
+      </c>
       <c r="AH111" s="5"/>
       <c r="AI111" s="5"/>
-      <c r="AJ111" s="5"/>
-      <c r="AK111" s="5"/>
-      <c r="AL111" s="5"/>
-      <c r="AM111" s="5"/>
+      <c r="AJ111" s="22"/>
+      <c r="AK111" s="23"/>
+      <c r="AL111" s="23"/>
+      <c r="AM111" s="24" t="s">
+        <v>8</v>
+      </c>
       <c r="AN111" s="5"/>
       <c r="AO111" s="5"/>
       <c r="AP111" s="5"/>
@@ -6127,19 +6021,45 @@
       <c r="BB111" s="4"/>
     </row>
     <row r="112" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A112" s="11"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+      <c r="H112" s="5"/>
+      <c r="I112" s="5"/>
+      <c r="J112" s="5"/>
+      <c r="K112" s="5"/>
+      <c r="L112" s="5"/>
+      <c r="M112" s="5"/>
+      <c r="N112" s="5"/>
+      <c r="O112" s="5"/>
+      <c r="P112" s="5"/>
+      <c r="Q112" s="5"/>
+      <c r="R112" s="5"/>
+      <c r="S112" s="5"/>
+      <c r="T112" s="5"/>
+      <c r="U112" s="5"/>
+      <c r="V112" s="5"/>
+      <c r="W112" s="5"/>
+      <c r="X112" s="5"/>
+      <c r="Y112" s="5"/>
+      <c r="Z112" s="4"/>
       <c r="AC112" s="11"/>
       <c r="AD112" s="5"/>
       <c r="AE112" s="5"/>
       <c r="AF112" s="5"/>
       <c r="AG112" s="5"/>
       <c r="AH112" s="5"/>
-      <c r="AI112" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="AJ112" s="33"/>
-      <c r="AK112" s="23"/>
-      <c r="AL112" s="23"/>
-      <c r="AM112" s="24"/>
+      <c r="AI112" s="5"/>
+      <c r="AJ112" s="5"/>
+      <c r="AK112" s="5"/>
+      <c r="AL112" s="5"/>
+      <c r="AM112" s="5"/>
       <c r="AN112" s="5"/>
       <c r="AO112" s="5"/>
       <c r="AP112" s="5"/>
@@ -6156,33 +6076,572 @@
       <c r="BA112" s="5"/>
       <c r="BB112" s="4"/>
     </row>
-    <row r="113" spans="29:54" x14ac:dyDescent="0.25">
-      <c r="AC113" s="3"/>
-      <c r="AD113" s="2"/>
-      <c r="AE113" s="2"/>
-      <c r="AF113" s="2"/>
-      <c r="AG113" s="2"/>
-      <c r="AH113" s="2"/>
-      <c r="AI113" s="2"/>
-      <c r="AJ113" s="2"/>
-      <c r="AK113" s="2"/>
-      <c r="AL113" s="2"/>
-      <c r="AM113" s="2"/>
-      <c r="AN113" s="2"/>
-      <c r="AO113" s="2"/>
-      <c r="AP113" s="2"/>
-      <c r="AQ113" s="2"/>
-      <c r="AR113" s="2"/>
-      <c r="AS113" s="2"/>
-      <c r="AT113" s="2"/>
-      <c r="AU113" s="2"/>
-      <c r="AV113" s="2"/>
-      <c r="AW113" s="2"/>
-      <c r="AX113" s="2"/>
-      <c r="AY113" s="2"/>
-      <c r="AZ113" s="2"/>
-      <c r="BA113" s="2"/>
-      <c r="BB113" s="1"/>
+    <row r="113" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A113" s="11"/>
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+      <c r="H113" s="5"/>
+      <c r="I113" s="5"/>
+      <c r="J113" s="5"/>
+      <c r="K113" s="5"/>
+      <c r="L113" s="5"/>
+      <c r="M113" s="5"/>
+      <c r="N113" s="5"/>
+      <c r="O113" s="5"/>
+      <c r="P113" s="5"/>
+      <c r="Q113" s="5"/>
+      <c r="R113" s="5"/>
+      <c r="S113" s="5"/>
+      <c r="T113" s="5"/>
+      <c r="U113" s="5"/>
+      <c r="V113" s="5"/>
+      <c r="W113" s="5"/>
+      <c r="X113" s="5"/>
+      <c r="Y113" s="5"/>
+      <c r="Z113" s="4"/>
+      <c r="AC113" s="11"/>
+      <c r="AD113" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE113" s="5"/>
+      <c r="AF113" s="5"/>
+      <c r="AG113" s="5"/>
+      <c r="AH113" s="5"/>
+      <c r="AI113" s="5"/>
+      <c r="AJ113" s="5"/>
+      <c r="AK113" s="5"/>
+      <c r="AL113" s="5"/>
+      <c r="AM113" s="5"/>
+      <c r="AN113" s="5"/>
+      <c r="AO113" s="5"/>
+      <c r="AP113" s="5"/>
+      <c r="AQ113" s="5"/>
+      <c r="AR113" s="5"/>
+      <c r="AS113" s="5"/>
+      <c r="AT113" s="5"/>
+      <c r="AU113" s="5"/>
+      <c r="AV113" s="5"/>
+      <c r="AW113" s="5"/>
+      <c r="AX113" s="5"/>
+      <c r="AY113" s="5"/>
+      <c r="AZ113" s="5"/>
+      <c r="BA113" s="5"/>
+      <c r="BB113" s="4"/>
+    </row>
+    <row r="114" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A114" s="11"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F114" s="33"/>
+      <c r="G114" s="23"/>
+      <c r="H114" s="23"/>
+      <c r="I114" s="24"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="5"/>
+      <c r="L114" s="5"/>
+      <c r="M114" s="5"/>
+      <c r="N114" s="5"/>
+      <c r="O114" s="5"/>
+      <c r="P114" s="5"/>
+      <c r="Q114" s="5"/>
+      <c r="R114" s="5"/>
+      <c r="S114" s="5"/>
+      <c r="T114" s="5"/>
+      <c r="U114" s="5"/>
+      <c r="V114" s="5"/>
+      <c r="W114" s="5"/>
+      <c r="X114" s="5"/>
+      <c r="Y114" s="5"/>
+      <c r="Z114" s="4"/>
+      <c r="AC114" s="11"/>
+      <c r="AD114" s="2"/>
+      <c r="AE114" s="2"/>
+      <c r="AF114" s="2"/>
+      <c r="AG114" s="2"/>
+      <c r="AH114" s="2"/>
+      <c r="AI114" s="2"/>
+      <c r="AJ114" s="5"/>
+      <c r="AK114" s="5"/>
+      <c r="AL114" s="5"/>
+      <c r="AM114" s="5"/>
+      <c r="AN114" s="5"/>
+      <c r="AO114" s="5"/>
+      <c r="AP114" s="5"/>
+      <c r="AQ114" s="5"/>
+      <c r="AR114" s="5"/>
+      <c r="AS114" s="5"/>
+      <c r="AT114" s="5"/>
+      <c r="AU114" s="5"/>
+      <c r="AV114" s="5"/>
+      <c r="AW114" s="5"/>
+      <c r="AX114" s="5"/>
+      <c r="AY114" s="5"/>
+      <c r="AZ114" s="5"/>
+      <c r="BA114" s="5"/>
+      <c r="BB114" s="4"/>
+    </row>
+    <row r="115" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A115" s="11"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="5"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5"/>
+      <c r="L115" s="5"/>
+      <c r="M115" s="5"/>
+      <c r="N115" s="5"/>
+      <c r="O115" s="5"/>
+      <c r="P115" s="5"/>
+      <c r="Q115" s="5"/>
+      <c r="R115" s="5"/>
+      <c r="S115" s="5"/>
+      <c r="T115" s="5"/>
+      <c r="U115" s="5"/>
+      <c r="V115" s="5"/>
+      <c r="W115" s="5"/>
+      <c r="X115" s="5"/>
+      <c r="Y115" s="5"/>
+      <c r="Z115" s="4"/>
+      <c r="AC115" s="11"/>
+      <c r="AD115" s="5"/>
+      <c r="AE115" s="5"/>
+      <c r="AF115" s="5"/>
+      <c r="AG115" s="5"/>
+      <c r="AH115" s="5"/>
+      <c r="AI115" s="5"/>
+      <c r="AJ115" s="5"/>
+      <c r="AK115" s="5"/>
+      <c r="AL115" s="5"/>
+      <c r="AM115" s="5"/>
+      <c r="AN115" s="5"/>
+      <c r="AO115" s="5"/>
+      <c r="AP115" s="5"/>
+      <c r="AQ115" s="5"/>
+      <c r="AR115" s="5"/>
+      <c r="AS115" s="5"/>
+      <c r="AT115" s="5"/>
+      <c r="AU115" s="5"/>
+      <c r="AV115" s="5"/>
+      <c r="AW115" s="5"/>
+      <c r="AX115" s="5"/>
+      <c r="AY115" s="5"/>
+      <c r="AZ115" s="5"/>
+      <c r="BA115" s="5"/>
+      <c r="BB115" s="4"/>
+    </row>
+    <row r="116" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A116" s="11"/>
+      <c r="B116" s="5"/>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="5"/>
+      <c r="I116" s="5"/>
+      <c r="J116" s="5"/>
+      <c r="K116" s="5"/>
+      <c r="L116" s="5"/>
+      <c r="M116" s="5"/>
+      <c r="N116" s="5"/>
+      <c r="O116" s="5"/>
+      <c r="P116" s="5"/>
+      <c r="Q116" s="5"/>
+      <c r="R116" s="5"/>
+      <c r="S116" s="5"/>
+      <c r="T116" s="5"/>
+      <c r="U116" s="5"/>
+      <c r="V116" s="5"/>
+      <c r="W116" s="5"/>
+      <c r="X116" s="5"/>
+      <c r="Y116" s="5"/>
+      <c r="Z116" s="4"/>
+      <c r="AC116" s="11"/>
+      <c r="AD116" s="5"/>
+      <c r="AE116" s="5"/>
+      <c r="AF116" s="5"/>
+      <c r="AG116" s="5"/>
+      <c r="AH116" s="5"/>
+      <c r="AI116" s="5"/>
+      <c r="AJ116" s="5"/>
+      <c r="AK116" s="5"/>
+      <c r="AL116" s="5"/>
+      <c r="AM116" s="5"/>
+      <c r="AN116" s="5"/>
+      <c r="AO116" s="5"/>
+      <c r="AP116" s="5"/>
+      <c r="AQ116" s="5"/>
+      <c r="AR116" s="5"/>
+      <c r="AS116" s="5"/>
+      <c r="AT116" s="5"/>
+      <c r="AU116" s="5"/>
+      <c r="AV116" s="5"/>
+      <c r="AW116" s="5"/>
+      <c r="AX116" s="5"/>
+      <c r="AY116" s="5"/>
+      <c r="AZ116" s="5"/>
+      <c r="BA116" s="5"/>
+      <c r="BB116" s="4"/>
+    </row>
+    <row r="117" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A117" s="3"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" s="2"/>
+      <c r="P117" s="2"/>
+      <c r="Q117" s="2"/>
+      <c r="R117" s="2"/>
+      <c r="S117" s="2"/>
+      <c r="T117" s="2"/>
+      <c r="U117" s="2"/>
+      <c r="V117" s="2"/>
+      <c r="W117" s="2"/>
+      <c r="X117" s="2"/>
+      <c r="Y117" s="2"/>
+      <c r="Z117" s="1"/>
+      <c r="AC117" s="11"/>
+      <c r="AD117" s="28"/>
+      <c r="AE117" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF117" s="2"/>
+      <c r="AG117" s="2"/>
+      <c r="AH117" s="2"/>
+      <c r="AI117" s="2"/>
+      <c r="AJ117" s="2"/>
+      <c r="AK117" s="2"/>
+      <c r="AL117" s="5"/>
+      <c r="AM117" s="5"/>
+      <c r="AN117" s="5"/>
+      <c r="AO117" s="5"/>
+      <c r="AP117" s="5"/>
+      <c r="AQ117" s="5"/>
+      <c r="AR117" s="5"/>
+      <c r="AS117" s="5"/>
+      <c r="AT117" s="5"/>
+      <c r="AU117" s="5"/>
+      <c r="AV117" s="5"/>
+      <c r="AW117" s="5"/>
+      <c r="AX117" s="5"/>
+      <c r="AY117" s="5"/>
+      <c r="AZ117" s="5"/>
+      <c r="BA117" s="5"/>
+      <c r="BB117" s="4"/>
+    </row>
+    <row r="118" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC118" s="11"/>
+      <c r="AD118" s="5"/>
+      <c r="AE118" s="5"/>
+      <c r="AF118" s="5"/>
+      <c r="AG118" s="5"/>
+      <c r="AH118" s="5"/>
+      <c r="AI118" s="5"/>
+      <c r="AJ118" s="5"/>
+      <c r="AK118" s="5"/>
+      <c r="AL118" s="5"/>
+      <c r="AM118" s="5"/>
+      <c r="AN118" s="5"/>
+      <c r="AO118" s="5"/>
+      <c r="AP118" s="5"/>
+      <c r="AQ118" s="5"/>
+      <c r="AR118" s="5"/>
+      <c r="AS118" s="5"/>
+      <c r="AT118" s="5"/>
+      <c r="AU118" s="5"/>
+      <c r="AV118" s="5"/>
+      <c r="AW118" s="5"/>
+      <c r="AX118" s="5"/>
+      <c r="AY118" s="5"/>
+      <c r="AZ118" s="5"/>
+      <c r="BA118" s="5"/>
+      <c r="BB118" s="4"/>
+    </row>
+    <row r="119" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC119" s="11"/>
+      <c r="AD119" s="28"/>
+      <c r="AE119" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF119" s="2"/>
+      <c r="AG119" s="2"/>
+      <c r="AH119" s="2"/>
+      <c r="AI119" s="2"/>
+      <c r="AJ119" s="2"/>
+      <c r="AK119" s="2"/>
+      <c r="AL119" s="5"/>
+      <c r="AM119" s="5"/>
+      <c r="AN119" s="5"/>
+      <c r="AO119" s="5"/>
+      <c r="AP119" s="5"/>
+      <c r="AQ119" s="5"/>
+      <c r="AR119" s="5"/>
+      <c r="AS119" s="5"/>
+      <c r="AT119" s="5"/>
+      <c r="AU119" s="5"/>
+      <c r="AV119" s="5"/>
+      <c r="AW119" s="5"/>
+      <c r="AX119" s="5"/>
+      <c r="AY119" s="5"/>
+      <c r="AZ119" s="5"/>
+      <c r="BA119" s="5"/>
+      <c r="BB119" s="4"/>
+    </row>
+    <row r="120" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC120" s="11"/>
+      <c r="AD120" s="5"/>
+      <c r="AE120" s="5"/>
+      <c r="AF120" s="5"/>
+      <c r="AG120" s="5"/>
+      <c r="AH120" s="5"/>
+      <c r="AI120" s="5"/>
+      <c r="AJ120" s="5"/>
+      <c r="AK120" s="5"/>
+      <c r="AL120" s="5"/>
+      <c r="AM120" s="5"/>
+      <c r="AN120" s="5"/>
+      <c r="AO120" s="5"/>
+      <c r="AP120" s="5"/>
+      <c r="AQ120" s="5"/>
+      <c r="AR120" s="5"/>
+      <c r="AS120" s="5"/>
+      <c r="AT120" s="5"/>
+      <c r="AU120" s="5"/>
+      <c r="AV120" s="5"/>
+      <c r="AW120" s="5"/>
+      <c r="AX120" s="5"/>
+      <c r="AY120" s="5"/>
+      <c r="AZ120" s="5"/>
+      <c r="BA120" s="5"/>
+      <c r="BB120" s="4"/>
+    </row>
+    <row r="121" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="F121" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC121" s="11"/>
+      <c r="AD121" s="28"/>
+      <c r="AE121" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF121" s="2"/>
+      <c r="AG121" s="2"/>
+      <c r="AH121" s="2"/>
+      <c r="AI121" s="2"/>
+      <c r="AJ121" s="2"/>
+      <c r="AK121" s="2"/>
+      <c r="AL121" s="5"/>
+      <c r="AM121" s="5"/>
+      <c r="AN121" s="5"/>
+      <c r="AO121" s="5"/>
+      <c r="AP121" s="5"/>
+      <c r="AQ121" s="5"/>
+      <c r="AR121" s="5"/>
+      <c r="AS121" s="5"/>
+      <c r="AT121" s="5"/>
+      <c r="AU121" s="5"/>
+      <c r="AV121" s="5"/>
+      <c r="AW121" s="5"/>
+      <c r="AX121" s="5"/>
+      <c r="AY121" s="5"/>
+      <c r="AZ121" s="5"/>
+      <c r="BA121" s="5"/>
+      <c r="BB121" s="4"/>
+    </row>
+    <row r="122" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC122" s="11"/>
+      <c r="AD122" s="5"/>
+      <c r="AE122" s="5"/>
+      <c r="AF122" s="5"/>
+      <c r="AG122" s="5"/>
+      <c r="AH122" s="5"/>
+      <c r="AI122" s="5"/>
+      <c r="AJ122" s="5"/>
+      <c r="AK122" s="5"/>
+      <c r="AL122" s="5"/>
+      <c r="AM122" s="5"/>
+      <c r="AN122" s="5"/>
+      <c r="AO122" s="5"/>
+      <c r="AP122" s="5"/>
+      <c r="AQ122" s="5"/>
+      <c r="AR122" s="5"/>
+      <c r="AS122" s="5"/>
+      <c r="AT122" s="5"/>
+      <c r="AU122" s="5"/>
+      <c r="AV122" s="5"/>
+      <c r="AW122" s="5"/>
+      <c r="AX122" s="5"/>
+      <c r="AY122" s="5"/>
+      <c r="AZ122" s="5"/>
+      <c r="BA122" s="5"/>
+      <c r="BB122" s="4"/>
+    </row>
+    <row r="123" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC123" s="11"/>
+      <c r="AD123" s="28"/>
+      <c r="AE123" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF123" s="2"/>
+      <c r="AG123" s="2"/>
+      <c r="AH123" s="2"/>
+      <c r="AI123" s="2"/>
+      <c r="AJ123" s="2"/>
+      <c r="AK123" s="2"/>
+      <c r="AL123" s="5"/>
+      <c r="AM123" s="5"/>
+      <c r="AN123" s="5"/>
+      <c r="AO123" s="5"/>
+      <c r="AP123" s="5"/>
+      <c r="AQ123" s="5"/>
+      <c r="AR123" s="5"/>
+      <c r="AS123" s="5"/>
+      <c r="AT123" s="5"/>
+      <c r="AU123" s="5"/>
+      <c r="AV123" s="5"/>
+      <c r="AW123" s="5"/>
+      <c r="AX123" s="5"/>
+      <c r="AY123" s="5"/>
+      <c r="AZ123" s="5"/>
+      <c r="BA123" s="5"/>
+      <c r="BB123" s="4"/>
+    </row>
+    <row r="124" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC124" s="11"/>
+      <c r="AD124" s="5"/>
+      <c r="AE124" s="5"/>
+      <c r="AF124" s="5"/>
+      <c r="AG124" s="5"/>
+      <c r="AH124" s="5"/>
+      <c r="AI124" s="5"/>
+      <c r="AJ124" s="5"/>
+      <c r="AK124" s="5"/>
+      <c r="AL124" s="5"/>
+      <c r="AM124" s="5"/>
+      <c r="AN124" s="5"/>
+      <c r="AO124" s="5"/>
+      <c r="AP124" s="5"/>
+      <c r="AQ124" s="5"/>
+      <c r="AR124" s="5"/>
+      <c r="AS124" s="5"/>
+      <c r="AT124" s="5"/>
+      <c r="AU124" s="5"/>
+      <c r="AV124" s="5"/>
+      <c r="AW124" s="5"/>
+      <c r="AX124" s="5"/>
+      <c r="AY124" s="5"/>
+      <c r="AZ124" s="5"/>
+      <c r="BA124" s="5"/>
+      <c r="BB124" s="4"/>
+    </row>
+    <row r="125" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC125" s="11"/>
+      <c r="AD125" s="5"/>
+      <c r="AE125" s="5"/>
+      <c r="AF125" s="5"/>
+      <c r="AG125" s="5"/>
+      <c r="AH125" s="5"/>
+      <c r="AI125" s="5"/>
+      <c r="AJ125" s="5"/>
+      <c r="AK125" s="5"/>
+      <c r="AL125" s="5"/>
+      <c r="AM125" s="5"/>
+      <c r="AN125" s="5"/>
+      <c r="AO125" s="5"/>
+      <c r="AP125" s="5"/>
+      <c r="AQ125" s="5"/>
+      <c r="AR125" s="5"/>
+      <c r="AS125" s="5"/>
+      <c r="AT125" s="5"/>
+      <c r="AU125" s="5"/>
+      <c r="AV125" s="5"/>
+      <c r="AW125" s="5"/>
+      <c r="AX125" s="5"/>
+      <c r="AY125" s="5"/>
+      <c r="AZ125" s="5"/>
+      <c r="BA125" s="5"/>
+      <c r="BB125" s="4"/>
+    </row>
+    <row r="126" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC126" s="11"/>
+      <c r="AD126" s="5"/>
+      <c r="AE126" s="5"/>
+      <c r="AF126" s="5"/>
+      <c r="AG126" s="5"/>
+      <c r="AH126" s="5"/>
+      <c r="AI126" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ126" s="33"/>
+      <c r="AK126" s="23"/>
+      <c r="AL126" s="23"/>
+      <c r="AM126" s="24"/>
+      <c r="AN126" s="5"/>
+      <c r="AO126" s="5"/>
+      <c r="AP126" s="5"/>
+      <c r="AQ126" s="5"/>
+      <c r="AR126" s="5"/>
+      <c r="AS126" s="5"/>
+      <c r="AT126" s="5"/>
+      <c r="AU126" s="5"/>
+      <c r="AV126" s="5"/>
+      <c r="AW126" s="5"/>
+      <c r="AX126" s="5"/>
+      <c r="AY126" s="5"/>
+      <c r="AZ126" s="5"/>
+      <c r="BA126" s="5"/>
+      <c r="BB126" s="4"/>
+    </row>
+    <row r="127" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AC127" s="3"/>
+      <c r="AD127" s="2"/>
+      <c r="AE127" s="2"/>
+      <c r="AF127" s="2"/>
+      <c r="AG127" s="2"/>
+      <c r="AH127" s="2"/>
+      <c r="AI127" s="2"/>
+      <c r="AJ127" s="2"/>
+      <c r="AK127" s="2"/>
+      <c r="AL127" s="2"/>
+      <c r="AM127" s="2"/>
+      <c r="AN127" s="2"/>
+      <c r="AO127" s="2"/>
+      <c r="AP127" s="2"/>
+      <c r="AQ127" s="2"/>
+      <c r="AR127" s="2"/>
+      <c r="AS127" s="2"/>
+      <c r="AT127" s="2"/>
+      <c r="AU127" s="2"/>
+      <c r="AV127" s="2"/>
+      <c r="AW127" s="2"/>
+      <c r="AX127" s="2"/>
+      <c r="AY127" s="2"/>
+      <c r="AZ127" s="2"/>
+      <c r="BA127" s="2"/>
+      <c r="BB127" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11074,8 +11533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ128"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="AT83" sqref="AT83"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="Y68" sqref="Y68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13665,13 +14124,15 @@
         <v>64</v>
       </c>
       <c r="AP78" s="5"/>
-      <c r="AQ78" s="5"/>
-      <c r="AR78" s="5"/>
-      <c r="AS78" s="5"/>
-      <c r="AT78" s="5"/>
-      <c r="AU78" s="5"/>
-      <c r="AV78" s="5"/>
-      <c r="AW78" s="5"/>
+      <c r="AQ78" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="AR78" s="37"/>
+      <c r="AS78" s="37"/>
+      <c r="AT78" s="37"/>
+      <c r="AU78" s="37"/>
+      <c r="AV78" s="37"/>
+      <c r="AW78" s="37"/>
       <c r="AX78" s="5"/>
       <c r="AZ78" s="5"/>
       <c r="BA78" s="5"/>
@@ -13728,13 +14189,15 @@
       <c r="AN79" s="2"/>
       <c r="AO79" s="2"/>
       <c r="AP79" s="5"/>
-      <c r="AQ79" s="5"/>
-      <c r="AR79" s="5"/>
-      <c r="AS79" s="5"/>
-      <c r="AT79" s="5"/>
-      <c r="AU79" s="5"/>
-      <c r="AV79" s="5"/>
-      <c r="AW79" s="5"/>
+      <c r="AQ79" s="39"/>
+      <c r="AR79" s="40"/>
+      <c r="AS79" s="41"/>
+      <c r="AT79" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="AU79" s="39"/>
+      <c r="AV79" s="40"/>
+      <c r="AW79" s="41"/>
       <c r="AX79" s="5"/>
       <c r="AZ79" s="5"/>
       <c r="BA79" s="5"/>
@@ -13844,24 +14307,12 @@
       <c r="AD81" s="5"/>
       <c r="AE81" s="4"/>
       <c r="AH81" s="11"/>
-      <c r="AI81" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ81" s="5"/>
-      <c r="AK81" s="5"/>
-      <c r="AL81" s="5"/>
-      <c r="AM81" s="5"/>
-      <c r="AN81" s="5"/>
-      <c r="AO81" s="5"/>
-      <c r="AP81" s="5"/>
-      <c r="AQ81" s="5"/>
-      <c r="AR81" s="5"/>
-      <c r="AS81" s="5"/>
-      <c r="AT81" s="5"/>
-      <c r="AU81" s="5"/>
-      <c r="AV81" s="5"/>
-      <c r="AW81" s="5"/>
-      <c r="AX81" s="5"/>
+      <c r="AI81" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ81" s="42"/>
+      <c r="AK81" s="42"/>
+      <c r="AL81" s="42"/>
       <c r="AZ81" s="5"/>
       <c r="BA81" s="5"/>
       <c r="BB81" s="5"/>
@@ -13909,21 +14360,12 @@
       <c r="AD82" s="5"/>
       <c r="AE82" s="4"/>
       <c r="AH82" s="11"/>
-      <c r="AJ82" s="5"/>
-      <c r="AK82" s="5"/>
-      <c r="AL82" s="5"/>
-      <c r="AM82" s="5"/>
-      <c r="AN82" s="5"/>
-      <c r="AO82" s="5"/>
-      <c r="AP82" s="5"/>
-      <c r="AQ82" s="5"/>
-      <c r="AR82" s="5"/>
-      <c r="AS82" s="5"/>
-      <c r="AT82" s="5"/>
-      <c r="AU82" s="5"/>
-      <c r="AV82" s="5"/>
-      <c r="AW82" s="5"/>
-      <c r="AX82" s="5"/>
+      <c r="AI82" s="38"/>
+      <c r="AJ82" s="38"/>
+      <c r="AK82" s="42"/>
+      <c r="AL82" s="42" t="s">
+        <v>103</v>
+      </c>
       <c r="AZ82" s="5"/>
       <c r="BA82" s="5"/>
       <c r="BB82" s="5"/>
@@ -13969,22 +14411,24 @@
       <c r="AD83" s="5"/>
       <c r="AE83" s="4"/>
       <c r="AH83" s="11"/>
-      <c r="AI83" s="9"/>
-      <c r="AJ83" s="8"/>
-      <c r="AK83" s="8"/>
-      <c r="AL83" s="8"/>
-      <c r="AM83" s="8"/>
-      <c r="AN83" s="8"/>
-      <c r="AO83" s="8"/>
-      <c r="AP83" s="8"/>
-      <c r="AQ83" s="8"/>
-      <c r="AR83" s="8"/>
-      <c r="AS83" s="8"/>
-      <c r="AT83" s="8"/>
-      <c r="AU83" s="8"/>
-      <c r="AV83" s="8"/>
-      <c r="AW83" s="8"/>
-      <c r="AX83" s="7"/>
+      <c r="AI83" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ83" s="5"/>
+      <c r="AK83" s="5"/>
+      <c r="AL83" s="5"/>
+      <c r="AM83" s="5"/>
+      <c r="AN83" s="5"/>
+      <c r="AO83" s="5"/>
+      <c r="AP83" s="5"/>
+      <c r="AQ83" s="5"/>
+      <c r="AR83" s="5"/>
+      <c r="AS83" s="5"/>
+      <c r="AT83" s="5"/>
+      <c r="AU83" s="5"/>
+      <c r="AV83" s="5"/>
+      <c r="AW83" s="5"/>
+      <c r="AX83" s="5"/>
       <c r="AZ83" s="5"/>
       <c r="BA83" s="5"/>
       <c r="BB83" s="5"/>
@@ -14030,7 +14474,6 @@
       <c r="AD84" s="5"/>
       <c r="AE84" s="4"/>
       <c r="AH84" s="11"/>
-      <c r="AI84" s="11"/>
       <c r="AJ84" s="5"/>
       <c r="AK84" s="5"/>
       <c r="AL84" s="5"/>
@@ -14045,7 +14488,7 @@
       <c r="AU84" s="5"/>
       <c r="AV84" s="5"/>
       <c r="AW84" s="5"/>
-      <c r="AX84" s="4"/>
+      <c r="AX84" s="5"/>
       <c r="AZ84" s="5"/>
       <c r="BA84" s="5"/>
       <c r="BB84" s="5"/>
@@ -14091,22 +14534,22 @@
       <c r="AD85" s="5"/>
       <c r="AE85" s="4"/>
       <c r="AH85" s="11"/>
-      <c r="AI85" s="11"/>
-      <c r="AJ85" s="5"/>
-      <c r="AK85" s="5"/>
-      <c r="AL85" s="5"/>
-      <c r="AM85" s="5"/>
-      <c r="AN85" s="5"/>
-      <c r="AO85" s="5"/>
-      <c r="AP85" s="5"/>
-      <c r="AQ85" s="5"/>
-      <c r="AR85" s="5"/>
-      <c r="AS85" s="5"/>
-      <c r="AT85" s="5"/>
-      <c r="AU85" s="5"/>
-      <c r="AV85" s="5"/>
-      <c r="AW85" s="5"/>
-      <c r="AX85" s="4"/>
+      <c r="AI85" s="9"/>
+      <c r="AJ85" s="8"/>
+      <c r="AK85" s="8"/>
+      <c r="AL85" s="8"/>
+      <c r="AM85" s="8"/>
+      <c r="AN85" s="8"/>
+      <c r="AO85" s="8"/>
+      <c r="AP85" s="8"/>
+      <c r="AQ85" s="8"/>
+      <c r="AR85" s="8"/>
+      <c r="AS85" s="8"/>
+      <c r="AT85" s="8"/>
+      <c r="AU85" s="8"/>
+      <c r="AV85" s="8"/>
+      <c r="AW85" s="8"/>
+      <c r="AX85" s="7"/>
       <c r="AZ85" s="5"/>
       <c r="BA85" s="5"/>
       <c r="BB85" s="5"/>
@@ -14154,22 +14597,22 @@
       <c r="AD86" s="5"/>
       <c r="AE86" s="4"/>
       <c r="AH86" s="11"/>
-      <c r="AI86" s="3"/>
-      <c r="AJ86" s="2"/>
-      <c r="AK86" s="2"/>
-      <c r="AL86" s="2"/>
-      <c r="AM86" s="2"/>
-      <c r="AN86" s="2"/>
-      <c r="AO86" s="2"/>
-      <c r="AP86" s="2"/>
-      <c r="AQ86" s="2"/>
-      <c r="AR86" s="2"/>
-      <c r="AS86" s="2"/>
-      <c r="AT86" s="2"/>
-      <c r="AU86" s="2"/>
-      <c r="AV86" s="2"/>
-      <c r="AW86" s="2"/>
-      <c r="AX86" s="1"/>
+      <c r="AI86" s="11"/>
+      <c r="AJ86" s="5"/>
+      <c r="AK86" s="5"/>
+      <c r="AL86" s="5"/>
+      <c r="AM86" s="5"/>
+      <c r="AN86" s="5"/>
+      <c r="AO86" s="5"/>
+      <c r="AP86" s="5"/>
+      <c r="AQ86" s="5"/>
+      <c r="AR86" s="5"/>
+      <c r="AS86" s="5"/>
+      <c r="AT86" s="5"/>
+      <c r="AU86" s="5"/>
+      <c r="AV86" s="5"/>
+      <c r="AW86" s="5"/>
+      <c r="AX86" s="4"/>
       <c r="AZ86" s="5"/>
       <c r="BA86" s="5"/>
       <c r="BB86" s="5"/>
@@ -14215,6 +14658,22 @@
       <c r="AD87" s="5"/>
       <c r="AE87" s="4"/>
       <c r="AH87" s="11"/>
+      <c r="AI87" s="11"/>
+      <c r="AJ87" s="5"/>
+      <c r="AK87" s="5"/>
+      <c r="AL87" s="5"/>
+      <c r="AM87" s="5"/>
+      <c r="AN87" s="5"/>
+      <c r="AO87" s="5"/>
+      <c r="AP87" s="5"/>
+      <c r="AQ87" s="5"/>
+      <c r="AR87" s="5"/>
+      <c r="AS87" s="5"/>
+      <c r="AT87" s="5"/>
+      <c r="AU87" s="5"/>
+      <c r="AV87" s="5"/>
+      <c r="AW87" s="5"/>
+      <c r="AX87" s="4"/>
       <c r="AZ87" s="5"/>
       <c r="BA87" s="5"/>
       <c r="BB87" s="5"/>
@@ -14262,6 +14721,22 @@
       <c r="AD88" s="5"/>
       <c r="AE88" s="4"/>
       <c r="AH88" s="11"/>
+      <c r="AI88" s="3"/>
+      <c r="AJ88" s="2"/>
+      <c r="AK88" s="2"/>
+      <c r="AL88" s="2"/>
+      <c r="AM88" s="2"/>
+      <c r="AN88" s="2"/>
+      <c r="AO88" s="2"/>
+      <c r="AP88" s="2"/>
+      <c r="AQ88" s="2"/>
+      <c r="AR88" s="2"/>
+      <c r="AS88" s="2"/>
+      <c r="AT88" s="2"/>
+      <c r="AU88" s="2"/>
+      <c r="AV88" s="2"/>
+      <c r="AW88" s="2"/>
+      <c r="AX88" s="1"/>
       <c r="AZ88" s="5"/>
       <c r="BA88" s="5"/>
       <c r="BB88" s="5"/>
@@ -14307,11 +14782,6 @@
       <c r="AD89" s="5"/>
       <c r="AE89" s="4"/>
       <c r="AH89" s="11"/>
-      <c r="AI89" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ89" s="23"/>
-      <c r="AK89" s="24"/>
       <c r="AZ89" s="5"/>
       <c r="BA89" s="5"/>
       <c r="BB89" s="5"/>
@@ -14402,6 +14872,11 @@
       <c r="AD91" s="5"/>
       <c r="AE91" s="4"/>
       <c r="AH91" s="11"/>
+      <c r="AI91" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ91" s="23"/>
+      <c r="AK91" s="24"/>
       <c r="AZ91" s="5"/>
       <c r="BA91" s="5"/>
       <c r="BB91" s="5"/>
@@ -16327,4 +16802,625 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AS32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="7"/>
+    </row>
+    <row r="2" spans="1:36" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="4"/>
+    </row>
+    <row r="3" spans="1:36" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="4"/>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="14"/>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="16"/>
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="16"/>
+      <c r="AG6" s="17"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
+      <c r="B7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+      <c r="AG7" s="17"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="19"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="19"/>
+      <c r="AE8" s="19"/>
+      <c r="AF8" s="19"/>
+      <c r="AG8" s="20"/>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="C10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" t="s">
+        <v>10</v>
+      </c>
+      <c r="R10" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="24"/>
+      <c r="Y10" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
+      <c r="AB10" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC10" s="56"/>
+      <c r="AD10" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH10" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="AI10" s="25"/>
+      <c r="AJ10" s="26"/>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="B24" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="24"/>
+      <c r="P24" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q24" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="24"/>
+      <c r="X24" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y24" s="54"/>
+      <c r="Z24" s="54"/>
+      <c r="AA24" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB24" s="56"/>
+      <c r="AC24" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD24" s="23"/>
+      <c r="AE24" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG24" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH24" s="23"/>
+      <c r="AI24" s="23"/>
+      <c r="AJ24" s="24"/>
+      <c r="AK24" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL24" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM24" s="23"/>
+      <c r="AN24" s="23"/>
+      <c r="AO24" s="24"/>
+      <c r="AQ24" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="AR24" s="25"/>
+      <c r="AS24" s="26"/>
+    </row>
+    <row r="27" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C27" s="9"/>
+      <c r="D27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="7"/>
+    </row>
+    <row r="28" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C28" s="11"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="4"/>
+    </row>
+    <row r="29" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C29" s="11"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="4"/>
+    </row>
+    <row r="30" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C30" s="11"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="4"/>
+    </row>
+    <row r="31" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C31" s="11"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="4"/>
+    </row>
+    <row r="32" spans="2:45" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
penambahan spec di kuningin
</commit_message>
<xml_diff>
--- a/document/Main Page.xlsx
+++ b/document/Main Page.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="118">
   <si>
     <t>LOGO</t>
   </si>
@@ -358,6 +358,21 @@
   <si>
     <t>harus ad aprofile untuk dari si tour(nama tour,nomor tlp,alamat),ini akan selalu tampil walaupun user pilih album atau ganti ke itenary</t>
   </si>
+  <si>
+    <t>Min Pax</t>
+  </si>
+  <si>
+    <t>Itenary Vendor</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>Harga</t>
+  </si>
+  <si>
+    <t>Itenary</t>
+  </si>
 </sst>
 </file>
 
@@ -560,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -618,6 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2084,7 +2100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB127"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:AK10"/>
     </sheetView>
   </sheetViews>
@@ -11533,7 +11549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ128"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="Y68" sqref="Y68"/>
     </sheetView>
   </sheetViews>
@@ -16806,10 +16822,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS32"/>
+  <dimension ref="A1:AS46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17328,11 +17344,15 @@
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
-      <c r="R27" s="7"/>
+      <c r="R27" s="7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="28" spans="2:45" x14ac:dyDescent="0.25">
       <c r="C28" s="11"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="57" t="s">
+        <v>115</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -17420,7 +17440,41 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="1"/>
     </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>109</v>
+      </c>
+      <c r="J40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
generate table dan spec
</commit_message>
<xml_diff>
--- a/document/Main Page.xlsx
+++ b/document/Main Page.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Tour" sheetId="3" r:id="rId3"/>
     <sheet name="Admin" sheetId="4" r:id="rId4"/>
     <sheet name="public vendor" sheetId="5" r:id="rId5"/>
+    <sheet name="Itenary Page" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="134">
   <si>
     <t>LOGO</t>
   </si>
@@ -372,6 +373,54 @@
   </si>
   <si>
     <t>Itenary</t>
+  </si>
+  <si>
+    <t>Profile tournya</t>
+  </si>
+  <si>
+    <t>isinya</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>no tlp</t>
+  </si>
+  <si>
+    <t>tombol ask itenary</t>
+  </si>
+  <si>
+    <t>tombol photo album</t>
+  </si>
+  <si>
+    <t>judul itenary</t>
+  </si>
+  <si>
+    <t>min pax</t>
+  </si>
+  <si>
+    <t>Negara kota</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tgl awa </t>
+  </si>
+  <si>
+    <t>tgl akhir</t>
+  </si>
+  <si>
+    <t>harga per pax</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>susunannya tlg diatur aja mar</t>
   </si>
 </sst>
 </file>
@@ -2100,7 +2149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB127"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:AK10"/>
     </sheetView>
   </sheetViews>
@@ -16824,8 +16873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17477,4 +17526,584 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="7"/>
+    </row>
+    <row r="2" spans="1:33" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="4"/>
+    </row>
+    <row r="3" spans="1:33" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="4"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="4"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="7"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="4"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="4"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG8" s="4"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="1"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="4"/>
+      <c r="M11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="4"/>
+      <c r="M13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="4"/>
+      <c r="M17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
create ulang table tr050 dan spec main page ada catatatn dikuningin
</commit_message>
<xml_diff>
--- a/document/Main Page.xlsx
+++ b/document/Main Page.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Main Page" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="147">
   <si>
     <t>LOGO</t>
   </si>
@@ -421,6 +421,45 @@
   </si>
   <si>
     <t>susunannya tlg diatur aja mar</t>
+  </si>
+  <si>
+    <t>diganti jadi isinya cm nama pacakge sama bawahnya</t>
+  </si>
+  <si>
+    <t>pake harga dan periode brangkat</t>
+  </si>
+  <si>
+    <t>dihapus/hidden</t>
+  </si>
+  <si>
+    <t>Email*</t>
+  </si>
+  <si>
+    <t>Password*</t>
+  </si>
+  <si>
+    <t>First Name*</t>
+  </si>
+  <si>
+    <t>Last Name*</t>
+  </si>
+  <si>
+    <t>Country*</t>
+  </si>
+  <si>
+    <t>City*</t>
+  </si>
+  <si>
+    <t>Phone Number*</t>
+  </si>
+  <si>
+    <t>Tour Travel Name*</t>
+  </si>
+  <si>
+    <t>Address*</t>
+  </si>
+  <si>
+    <t>Zip Code*</t>
   </si>
 </sst>
 </file>
@@ -871,6 +910,100 @@
         <a:xfrm>
           <a:off x="1571625" y="22802850"/>
           <a:ext cx="0" cy="1009650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8801100" y="4495800"/>
+          <a:ext cx="695325" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8791575" y="2514600"/>
+          <a:ext cx="695325" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2149,8 +2282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB127"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:AK10"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ16" sqref="AQ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,7 +2291,7 @@
     <col min="1" max="256" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -2193,7 +2326,7 @@
       <c r="AF1" s="8"/>
       <c r="AG1" s="7"/>
     </row>
-    <row r="2" spans="1:38" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:43" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2363,7 @@
       <c r="AF2" s="5"/>
       <c r="AG2" s="4"/>
     </row>
-    <row r="3" spans="1:38" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:43" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2265,7 +2398,7 @@
       <c r="AF3" s="5"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2307,7 +2440,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2342,7 +2475,7 @@
       <c r="AF5" s="13"/>
       <c r="AG5" s="14"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
       <c r="B6" s="16" t="s">
         <v>3</v>
@@ -2379,7 +2512,7 @@
       <c r="AF6" s="16"/>
       <c r="AG6" s="17"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
         <v>4</v>
@@ -2416,7 +2549,7 @@
       <c r="AF7" s="16"/>
       <c r="AG7" s="17"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
         <v>5</v>
@@ -2456,7 +2589,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>6</v>
       </c>
@@ -2514,12 +2647,12 @@
       <c r="AJ10" s="25"/>
       <c r="AK10" s="26"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="AD11" s="16"/>
       <c r="AE11" s="16"/>
       <c r="AF11" s="16"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -2559,8 +2692,14 @@
       <c r="AH12" s="8"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="7"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AN12" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO12" s="42"/>
+      <c r="AP12" s="42"/>
+      <c r="AQ12" s="42"/>
+    </row>
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2595,7 +2734,7 @@
       <c r="AI13" s="5"/>
       <c r="AJ13" s="4"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2630,7 +2769,7 @@
       <c r="AI14" s="5"/>
       <c r="AJ14" s="4"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2665,7 +2804,7 @@
       <c r="AI15" s="5"/>
       <c r="AJ15" s="4"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
@@ -2706,7 +2845,7 @@
       <c r="AI16" s="5"/>
       <c r="AJ16" s="4"/>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2741,7 +2880,7 @@
       <c r="AI17" s="5"/>
       <c r="AJ17" s="4"/>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2776,7 +2915,7 @@
       <c r="AI18" s="5"/>
       <c r="AJ18" s="4"/>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2811,7 +2950,7 @@
       <c r="AI19" s="5"/>
       <c r="AJ19" s="4"/>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -2846,7 +2985,7 @@
       <c r="AI20" s="5"/>
       <c r="AJ20" s="4"/>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2881,7 +3020,7 @@
       <c r="AI21" s="2"/>
       <c r="AJ21" s="1"/>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -2916,7 +3055,7 @@
       <c r="AI22" s="5"/>
       <c r="AJ22" s="4"/>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>15</v>
       </c>
@@ -2968,8 +3107,23 @@
       </c>
       <c r="AI23" s="5"/>
       <c r="AJ23" s="4"/>
-    </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN23" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="AO23" s="42"/>
+      <c r="AP23" s="42"/>
+      <c r="AQ23" s="42"/>
+      <c r="AR23" s="42"/>
+      <c r="AS23" s="42"/>
+      <c r="AT23" s="42"/>
+      <c r="AU23" s="42"/>
+      <c r="AV23" s="42"/>
+      <c r="AW23" s="42"/>
+      <c r="AX23" s="42"/>
+      <c r="AY23" s="42"/>
+      <c r="AZ23" s="42"/>
+    </row>
+    <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -3003,8 +3157,23 @@
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="1"/>
-    </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="AN24" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO24" s="42"/>
+      <c r="AP24" s="42"/>
+      <c r="AQ24" s="42"/>
+      <c r="AR24" s="42"/>
+      <c r="AS24" s="42"/>
+      <c r="AT24" s="42"/>
+      <c r="AU24" s="42"/>
+      <c r="AV24" s="42"/>
+      <c r="AW24" s="42"/>
+      <c r="AX24" s="42"/>
+      <c r="AY24" s="42"/>
+      <c r="AZ24" s="42"/>
+    </row>
+    <row r="27" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -3045,7 +3214,7 @@
       <c r="AI27" s="8"/>
       <c r="AJ27" s="7"/>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -3080,7 +3249,7 @@
       <c r="AI28" s="5"/>
       <c r="AJ28" s="4"/>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -3115,7 +3284,7 @@
       <c r="AI29" s="5"/>
       <c r="AJ29" s="4"/>
     </row>
-    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -3150,7 +3319,7 @@
       <c r="AI30" s="5"/>
       <c r="AJ30" s="4"/>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
@@ -3191,7 +3360,7 @@
       <c r="AI31" s="5"/>
       <c r="AJ31" s="4"/>
     </row>
-    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -6719,8 +6888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK156"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O164" sqref="O164"/>
+    <sheetView topLeftCell="A109" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7052,7 +7221,7 @@
       <c r="O11" s="7"/>
       <c r="P11" s="5"/>
       <c r="S11" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
@@ -7142,7 +7311,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="5"/>
       <c r="S14" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
@@ -7339,7 +7508,7 @@
       <c r="G21" s="11"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
@@ -7350,7 +7519,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
@@ -7671,7 +7840,7 @@
       <c r="G32" s="11"/>
       <c r="H32" s="5"/>
       <c r="I32" s="30" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
@@ -7679,7 +7848,7 @@
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="30" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
@@ -7766,7 +7935,7 @@
       <c r="G35" s="11"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>36</v>
+        <v>143</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
@@ -11598,8 +11767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ128"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="Y68" sqref="Y68"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11920,7 +12089,7 @@
       <c r="O12" s="7"/>
       <c r="P12" s="5"/>
       <c r="S12" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
@@ -11996,7 +12165,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="5"/>
       <c r="S15" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
@@ -12162,7 +12331,7 @@
     <row r="22" spans="2:33" x14ac:dyDescent="0.25">
       <c r="G22" s="11"/>
       <c r="H22" s="5" t="s">
-        <v>49</v>
+        <v>139</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -12173,7 +12342,7 @@
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
       <c r="Q22" s="5" t="s">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="R22" s="5"/>
       <c r="S22" s="5"/>
@@ -12282,7 +12451,7 @@
     <row r="26" spans="2:33" x14ac:dyDescent="0.25">
       <c r="G26" s="11"/>
       <c r="H26" s="5" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -12371,7 +12540,7 @@
     <row r="29" spans="2:33" x14ac:dyDescent="0.25">
       <c r="G29" s="11"/>
       <c r="H29" s="5" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -12518,7 +12687,7 @@
     <row r="34" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G34" s="11"/>
       <c r="H34" s="5" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -12607,7 +12776,7 @@
     <row r="37" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G37" s="11"/>
       <c r="H37" s="30" t="s">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
@@ -12615,7 +12784,7 @@
       <c r="L37" s="5"/>
       <c r="M37" s="5"/>
       <c r="N37" s="30" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
@@ -12702,7 +12871,7 @@
     <row r="40" spans="7:33" x14ac:dyDescent="0.25">
       <c r="G40" s="11"/>
       <c r="H40" s="5" t="s">
-        <v>36</v>
+        <v>143</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -16131,7 +16300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -17532,7 +17701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>

</xml_diff>